<commit_message>
[MS-OFFICIALFILE] Add 2 new cases and 5 capture code for 3 fixed TDIs\TDQs
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-OFFICIALFILE/MS-OFFICIALFILE_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-OFFICIALFILE/MS-OFFICIALFILE_RequirementSpecification.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17301"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Source Depot\Repos\Interop-TestSuites-1\SharePoint\Docs\MS-OFFICIALFILE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
   </bookViews>
@@ -3041,7 +3046,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -3996,7 +4001,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4029,9 +4034,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4064,6 +4086,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4243,21 +4282,19 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A375" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C377" sqref="C377"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="11" width="9" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
@@ -4598,7 +4635,7 @@
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="21" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A21" s="22" t="s">
         <v>45</v>
       </c>
@@ -4675,7 +4712,7 @@
       </c>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" ht="60">
+    <row r="24" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A24" s="22" t="s">
         <v>48</v>
       </c>
@@ -4700,7 +4737,7 @@
       </c>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" spans="1:12" s="23" customFormat="1" ht="60">
+    <row r="25" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A25" s="22" t="s">
         <v>49</v>
       </c>
@@ -4725,7 +4762,7 @@
       </c>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:12" s="23" customFormat="1" ht="60">
+    <row r="26" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A26" s="22" t="s">
         <v>50</v>
       </c>
@@ -4750,7 +4787,7 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="27" spans="1:12" s="23" customFormat="1">
       <c r="A27" s="22" t="s">
         <v>51</v>
       </c>
@@ -4875,7 +4912,7 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="32" spans="1:12" s="23" customFormat="1">
       <c r="A32" s="22" t="s">
         <v>56</v>
       </c>
@@ -4900,7 +4937,7 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" ht="30">
+    <row r="33" spans="1:9" s="23" customFormat="1">
       <c r="A33" s="22" t="s">
         <v>57</v>
       </c>
@@ -4950,7 +4987,7 @@
       </c>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:9" ht="45">
+    <row r="35" spans="1:9" ht="30">
       <c r="A35" s="30" t="s">
         <v>59</v>
       </c>
@@ -5025,7 +5062,7 @@
       </c>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" spans="1:9" ht="45">
+    <row r="38" spans="1:9" ht="30">
       <c r="A38" s="30" t="s">
         <v>62</v>
       </c>
@@ -5250,7 +5287,7 @@
       </c>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" spans="1:9" ht="150">
+    <row r="47" spans="1:9" ht="120">
       <c r="A47" s="30" t="s">
         <v>71</v>
       </c>
@@ -5275,7 +5312,7 @@
       </c>
       <c r="I47" s="32"/>
     </row>
-    <row r="48" spans="1:9" ht="30">
+    <row r="48" spans="1:9">
       <c r="A48" s="30" t="s">
         <v>72</v>
       </c>
@@ -5325,7 +5362,7 @@
       </c>
       <c r="I49" s="32"/>
     </row>
-    <row r="50" spans="1:9" ht="120">
+    <row r="50" spans="1:9" ht="90">
       <c r="A50" s="30" t="s">
         <v>74</v>
       </c>
@@ -5400,7 +5437,7 @@
       </c>
       <c r="I52" s="32"/>
     </row>
-    <row r="53" spans="1:9" ht="165">
+    <row r="53" spans="1:9" ht="150">
       <c r="A53" s="30" t="s">
         <v>77</v>
       </c>
@@ -5475,7 +5512,7 @@
       </c>
       <c r="I55" s="32"/>
     </row>
-    <row r="56" spans="1:9" ht="30">
+    <row r="56" spans="1:9">
       <c r="A56" s="30" t="s">
         <v>80</v>
       </c>
@@ -5500,7 +5537,7 @@
       </c>
       <c r="I56" s="32"/>
     </row>
-    <row r="57" spans="1:9" ht="30">
+    <row r="57" spans="1:9">
       <c r="A57" s="30" t="s">
         <v>81</v>
       </c>
@@ -5700,7 +5737,7 @@
       </c>
       <c r="I64" s="32"/>
     </row>
-    <row r="65" spans="1:9" ht="45">
+    <row r="65" spans="1:9" ht="30">
       <c r="A65" s="30" t="s">
         <v>89</v>
       </c>
@@ -5750,7 +5787,7 @@
       </c>
       <c r="I66" s="32"/>
     </row>
-    <row r="67" spans="1:9" ht="30">
+    <row r="67" spans="1:9">
       <c r="A67" s="30" t="s">
         <v>91</v>
       </c>
@@ -5800,7 +5837,7 @@
       </c>
       <c r="I68" s="32"/>
     </row>
-    <row r="69" spans="1:9" ht="30">
+    <row r="69" spans="1:9">
       <c r="A69" s="30" t="s">
         <v>93</v>
       </c>
@@ -5875,7 +5912,7 @@
       </c>
       <c r="I71" s="32"/>
     </row>
-    <row r="72" spans="1:9" ht="45">
+    <row r="72" spans="1:9" ht="30">
       <c r="A72" s="30" t="s">
         <v>96</v>
       </c>
@@ -6000,7 +6037,7 @@
       </c>
       <c r="I76" s="32"/>
     </row>
-    <row r="77" spans="1:9" ht="45">
+    <row r="77" spans="1:9" ht="30">
       <c r="A77" s="30" t="s">
         <v>101</v>
       </c>
@@ -6025,7 +6062,7 @@
       </c>
       <c r="I77" s="32"/>
     </row>
-    <row r="78" spans="1:9" ht="30">
+    <row r="78" spans="1:9">
       <c r="A78" s="30" t="s">
         <v>102</v>
       </c>
@@ -6300,7 +6337,7 @@
       </c>
       <c r="I88" s="32"/>
     </row>
-    <row r="89" spans="1:9" ht="60">
+    <row r="89" spans="1:9" ht="45">
       <c r="A89" s="30" t="s">
         <v>113</v>
       </c>
@@ -6327,7 +6364,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="30">
+    <row r="90" spans="1:9">
       <c r="A90" s="30" t="s">
         <v>114</v>
       </c>
@@ -6352,7 +6389,7 @@
       </c>
       <c r="I90" s="32"/>
     </row>
-    <row r="91" spans="1:9" ht="30">
+    <row r="91" spans="1:9">
       <c r="A91" s="30" t="s">
         <v>115</v>
       </c>
@@ -6377,7 +6414,7 @@
       </c>
       <c r="I91" s="32"/>
     </row>
-    <row r="92" spans="1:9" ht="195">
+    <row r="92" spans="1:9" ht="165">
       <c r="A92" s="30" t="s">
         <v>116</v>
       </c>
@@ -6602,7 +6639,7 @@
       </c>
       <c r="I100" s="32"/>
     </row>
-    <row r="101" spans="1:9" ht="30">
+    <row r="101" spans="1:9">
       <c r="A101" s="30" t="s">
         <v>125</v>
       </c>
@@ -6627,7 +6664,7 @@
       </c>
       <c r="I101" s="32"/>
     </row>
-    <row r="102" spans="1:9" ht="135">
+    <row r="102" spans="1:9" ht="120">
       <c r="A102" s="30" t="s">
         <v>126</v>
       </c>
@@ -6702,7 +6739,7 @@
       </c>
       <c r="I104" s="32"/>
     </row>
-    <row r="105" spans="1:9" ht="30">
+    <row r="105" spans="1:9">
       <c r="A105" s="30" t="s">
         <v>129</v>
       </c>
@@ -6723,7 +6760,7 @@
         <v>15</v>
       </c>
       <c r="H105" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I105" s="32"/>
     </row>
@@ -6748,11 +6785,11 @@
         <v>15</v>
       </c>
       <c r="H106" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I106" s="32"/>
     </row>
-    <row r="107" spans="1:9" ht="30">
+    <row r="107" spans="1:9">
       <c r="A107" s="30" t="s">
         <v>131</v>
       </c>
@@ -6777,7 +6814,7 @@
       </c>
       <c r="I107" s="32"/>
     </row>
-    <row r="108" spans="1:9" ht="210">
+    <row r="108" spans="1:9" ht="195">
       <c r="A108" s="30" t="s">
         <v>132</v>
       </c>
@@ -7127,7 +7164,7 @@
       </c>
       <c r="I121" s="32"/>
     </row>
-    <row r="122" spans="1:9" ht="30">
+    <row r="122" spans="1:9">
       <c r="A122" s="30" t="s">
         <v>146</v>
       </c>
@@ -7152,7 +7189,7 @@
       </c>
       <c r="I122" s="32"/>
     </row>
-    <row r="123" spans="1:9" ht="45">
+    <row r="123" spans="1:9" ht="30">
       <c r="A123" s="30" t="s">
         <v>147</v>
       </c>
@@ -7252,7 +7289,7 @@
       </c>
       <c r="I126" s="32"/>
     </row>
-    <row r="127" spans="1:9" ht="60">
+    <row r="127" spans="1:9" ht="45">
       <c r="A127" s="30" t="s">
         <v>151</v>
       </c>
@@ -7352,7 +7389,7 @@
       </c>
       <c r="I130" s="32"/>
     </row>
-    <row r="131" spans="1:9" ht="45">
+    <row r="131" spans="1:9" ht="30">
       <c r="A131" s="30" t="s">
         <v>155</v>
       </c>
@@ -7552,7 +7589,7 @@
       </c>
       <c r="I138" s="32"/>
     </row>
-    <row r="139" spans="1:9" ht="45">
+    <row r="139" spans="1:9" ht="30">
       <c r="A139" s="30" t="s">
         <v>163</v>
       </c>
@@ -7602,7 +7639,7 @@
       </c>
       <c r="I140" s="32"/>
     </row>
-    <row r="141" spans="1:9" ht="60">
+    <row r="141" spans="1:9" ht="45">
       <c r="A141" s="30" t="s">
         <v>165</v>
       </c>
@@ -7629,7 +7666,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="142" spans="1:9" ht="45">
+    <row r="142" spans="1:9" ht="30">
       <c r="A142" s="30" t="s">
         <v>166</v>
       </c>
@@ -7656,7 +7693,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="45">
+    <row r="143" spans="1:9" ht="30">
       <c r="A143" s="30" t="s">
         <v>167</v>
       </c>
@@ -7683,7 +7720,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="45">
+    <row r="144" spans="1:9" ht="30">
       <c r="A144" s="30" t="s">
         <v>168</v>
       </c>
@@ -7760,7 +7797,7 @@
       </c>
       <c r="I146" s="32"/>
     </row>
-    <row r="147" spans="1:9" ht="45">
+    <row r="147" spans="1:9" ht="30">
       <c r="A147" s="30" t="s">
         <v>171</v>
       </c>
@@ -7837,7 +7874,7 @@
       </c>
       <c r="I149" s="32"/>
     </row>
-    <row r="150" spans="1:9" ht="60">
+    <row r="150" spans="1:9" ht="45">
       <c r="A150" s="30" t="s">
         <v>173</v>
       </c>
@@ -7862,7 +7899,7 @@
       </c>
       <c r="I150" s="32"/>
     </row>
-    <row r="151" spans="1:9" ht="90">
+    <row r="151" spans="1:9" ht="75">
       <c r="A151" s="30" t="s">
         <v>174</v>
       </c>
@@ -7887,7 +7924,7 @@
       </c>
       <c r="I151" s="32"/>
     </row>
-    <row r="152" spans="1:9" ht="90">
+    <row r="152" spans="1:9" ht="75">
       <c r="A152" s="30" t="s">
         <v>175</v>
       </c>
@@ -7912,7 +7949,7 @@
       </c>
       <c r="I152" s="32"/>
     </row>
-    <row r="153" spans="1:9" ht="90">
+    <row r="153" spans="1:9" ht="75">
       <c r="A153" s="30" t="s">
         <v>176</v>
       </c>
@@ -8012,7 +8049,7 @@
       </c>
       <c r="I156" s="32"/>
     </row>
-    <row r="157" spans="1:9" ht="90">
+    <row r="157" spans="1:9" ht="75">
       <c r="A157" s="30" t="s">
         <v>180</v>
       </c>
@@ -8037,7 +8074,7 @@
       </c>
       <c r="I157" s="32"/>
     </row>
-    <row r="158" spans="1:9" ht="105">
+    <row r="158" spans="1:9" ht="90">
       <c r="A158" s="30" t="s">
         <v>181</v>
       </c>
@@ -8087,7 +8124,7 @@
       </c>
       <c r="I159" s="32"/>
     </row>
-    <row r="160" spans="1:9" ht="90">
+    <row r="160" spans="1:9" ht="75">
       <c r="A160" s="30" t="s">
         <v>183</v>
       </c>
@@ -8114,7 +8151,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="75">
+    <row r="161" spans="1:9" ht="60">
       <c r="A161" s="30" t="s">
         <v>184</v>
       </c>
@@ -8141,7 +8178,7 @@
       </c>
       <c r="I161" s="32"/>
     </row>
-    <row r="162" spans="1:9" ht="105">
+    <row r="162" spans="1:9" ht="90">
       <c r="A162" s="30" t="s">
         <v>185</v>
       </c>
@@ -8191,7 +8228,7 @@
       </c>
       <c r="I163" s="32"/>
     </row>
-    <row r="164" spans="1:9" ht="90">
+    <row r="164" spans="1:9" ht="75">
       <c r="A164" s="30" t="s">
         <v>187</v>
       </c>
@@ -8216,7 +8253,7 @@
       </c>
       <c r="I164" s="32"/>
     </row>
-    <row r="165" spans="1:9" ht="105">
+    <row r="165" spans="1:9" ht="90">
       <c r="A165" s="30" t="s">
         <v>188</v>
       </c>
@@ -8241,7 +8278,7 @@
       </c>
       <c r="I165" s="32"/>
     </row>
-    <row r="166" spans="1:9" ht="150">
+    <row r="166" spans="1:9" ht="120">
       <c r="A166" s="30" t="s">
         <v>189</v>
       </c>
@@ -8266,7 +8303,7 @@
       </c>
       <c r="I166" s="32"/>
     </row>
-    <row r="167" spans="1:9" ht="165">
+    <row r="167" spans="1:9" ht="135">
       <c r="A167" s="30" t="s">
         <v>190</v>
       </c>
@@ -8291,7 +8328,7 @@
       </c>
       <c r="I167" s="32"/>
     </row>
-    <row r="168" spans="1:9" ht="60">
+    <row r="168" spans="1:9" ht="45">
       <c r="A168" s="30" t="s">
         <v>191</v>
       </c>
@@ -8316,7 +8353,7 @@
       </c>
       <c r="I168" s="32"/>
     </row>
-    <row r="169" spans="1:9" ht="60">
+    <row r="169" spans="1:9" ht="45">
       <c r="A169" s="30" t="s">
         <v>192</v>
       </c>
@@ -8366,7 +8403,7 @@
       </c>
       <c r="I170" s="32"/>
     </row>
-    <row r="171" spans="1:9" ht="45">
+    <row r="171" spans="1:9" ht="30">
       <c r="A171" s="30" t="s">
         <v>194</v>
       </c>
@@ -8516,7 +8553,7 @@
       </c>
       <c r="I176" s="32"/>
     </row>
-    <row r="177" spans="1:9" ht="225">
+    <row r="177" spans="1:9" ht="195">
       <c r="A177" s="30" t="s">
         <v>200</v>
       </c>
@@ -8616,7 +8653,7 @@
       </c>
       <c r="I180" s="32"/>
     </row>
-    <row r="181" spans="1:9" ht="180">
+    <row r="181" spans="1:9" ht="165">
       <c r="A181" s="30" t="s">
         <v>204</v>
       </c>
@@ -8641,7 +8678,7 @@
       </c>
       <c r="I181" s="32"/>
     </row>
-    <row r="182" spans="1:9" ht="60">
+    <row r="182" spans="1:9" ht="45">
       <c r="A182" s="30" t="s">
         <v>205</v>
       </c>
@@ -8716,7 +8753,7 @@
       </c>
       <c r="I184" s="32"/>
     </row>
-    <row r="185" spans="1:9" ht="180">
+    <row r="185" spans="1:9" ht="150">
       <c r="A185" s="30" t="s">
         <v>208</v>
       </c>
@@ -8741,7 +8778,7 @@
       </c>
       <c r="I185" s="32"/>
     </row>
-    <row r="186" spans="1:9" ht="30">
+    <row r="186" spans="1:9">
       <c r="A186" s="30" t="s">
         <v>209</v>
       </c>
@@ -8791,7 +8828,7 @@
       </c>
       <c r="I187" s="32"/>
     </row>
-    <row r="188" spans="1:9" ht="45">
+    <row r="188" spans="1:9" ht="30">
       <c r="A188" s="30" t="s">
         <v>211</v>
       </c>
@@ -8816,7 +8853,7 @@
       </c>
       <c r="I188" s="32"/>
     </row>
-    <row r="189" spans="1:9" ht="45">
+    <row r="189" spans="1:9" ht="30">
       <c r="A189" s="30" t="s">
         <v>212</v>
       </c>
@@ -8891,7 +8928,7 @@
       </c>
       <c r="I191" s="32"/>
     </row>
-    <row r="192" spans="1:9" ht="240">
+    <row r="192" spans="1:9" ht="225">
       <c r="A192" s="30" t="s">
         <v>215</v>
       </c>
@@ -9066,7 +9103,7 @@
       </c>
       <c r="I198" s="32"/>
     </row>
-    <row r="199" spans="1:9" ht="45">
+    <row r="199" spans="1:9" ht="30">
       <c r="A199" s="30" t="s">
         <v>222</v>
       </c>
@@ -9116,7 +9153,7 @@
       </c>
       <c r="I200" s="32"/>
     </row>
-    <row r="201" spans="1:9" ht="45">
+    <row r="201" spans="1:9" ht="30">
       <c r="A201" s="30" t="s">
         <v>224</v>
       </c>
@@ -9141,7 +9178,7 @@
       </c>
       <c r="I201" s="32"/>
     </row>
-    <row r="202" spans="1:9" ht="45">
+    <row r="202" spans="1:9" ht="30">
       <c r="A202" s="30" t="s">
         <v>225</v>
       </c>
@@ -9166,7 +9203,7 @@
       </c>
       <c r="I202" s="32"/>
     </row>
-    <row r="203" spans="1:9" ht="30">
+    <row r="203" spans="1:9">
       <c r="A203" s="30" t="s">
         <v>226</v>
       </c>
@@ -9216,7 +9253,7 @@
       </c>
       <c r="I204" s="32"/>
     </row>
-    <row r="205" spans="1:9" ht="45">
+    <row r="205" spans="1:9" ht="30">
       <c r="A205" s="30" t="s">
         <v>228</v>
       </c>
@@ -9366,7 +9403,7 @@
       </c>
       <c r="I210" s="32"/>
     </row>
-    <row r="211" spans="1:9" ht="45">
+    <row r="211" spans="1:9" ht="30">
       <c r="A211" s="30" t="s">
         <v>234</v>
       </c>
@@ -9393,7 +9430,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="212" spans="1:9" ht="90">
+    <row r="212" spans="1:9" ht="75">
       <c r="A212" s="30" t="s">
         <v>235</v>
       </c>
@@ -9418,7 +9455,7 @@
       </c>
       <c r="I212" s="32"/>
     </row>
-    <row r="213" spans="1:9" ht="45">
+    <row r="213" spans="1:9" ht="30">
       <c r="A213" s="30" t="s">
         <v>236</v>
       </c>
@@ -9443,7 +9480,7 @@
       </c>
       <c r="I213" s="32"/>
     </row>
-    <row r="214" spans="1:9" ht="60">
+    <row r="214" spans="1:9" ht="45">
       <c r="A214" s="30" t="s">
         <v>237</v>
       </c>
@@ -9593,7 +9630,7 @@
       </c>
       <c r="I219" s="32"/>
     </row>
-    <row r="220" spans="1:9" ht="30">
+    <row r="220" spans="1:9">
       <c r="A220" s="30" t="s">
         <v>243</v>
       </c>
@@ -9643,7 +9680,7 @@
       </c>
       <c r="I221" s="32"/>
     </row>
-    <row r="222" spans="1:9" ht="45">
+    <row r="222" spans="1:9" ht="30">
       <c r="A222" s="30" t="s">
         <v>245</v>
       </c>
@@ -9693,7 +9730,7 @@
       </c>
       <c r="I223" s="32"/>
     </row>
-    <row r="224" spans="1:9" ht="75">
+    <row r="224" spans="1:9" ht="60">
       <c r="A224" s="30" t="s">
         <v>247</v>
       </c>
@@ -9718,7 +9755,7 @@
       </c>
       <c r="I224" s="32"/>
     </row>
-    <row r="225" spans="1:9" ht="165">
+    <row r="225" spans="1:9" ht="135">
       <c r="A225" s="30" t="s">
         <v>248</v>
       </c>
@@ -9768,7 +9805,7 @@
       </c>
       <c r="I226" s="32"/>
     </row>
-    <row r="227" spans="1:9" ht="45">
+    <row r="227" spans="1:9" ht="30">
       <c r="A227" s="30" t="s">
         <v>250</v>
       </c>
@@ -9793,7 +9830,7 @@
       </c>
       <c r="I227" s="32"/>
     </row>
-    <row r="228" spans="1:9" ht="45">
+    <row r="228" spans="1:9" ht="30">
       <c r="A228" s="30" t="s">
         <v>251</v>
       </c>
@@ -9818,7 +9855,7 @@
       </c>
       <c r="I228" s="32"/>
     </row>
-    <row r="229" spans="1:9" ht="30">
+    <row r="229" spans="1:9">
       <c r="A229" s="30" t="s">
         <v>252</v>
       </c>
@@ -9843,7 +9880,7 @@
       </c>
       <c r="I229" s="32"/>
     </row>
-    <row r="230" spans="1:9" ht="120">
+    <row r="230" spans="1:9" ht="105">
       <c r="A230" s="30" t="s">
         <v>253</v>
       </c>
@@ -9893,7 +9930,7 @@
       </c>
       <c r="I231" s="32"/>
     </row>
-    <row r="232" spans="1:9" ht="30">
+    <row r="232" spans="1:9">
       <c r="A232" s="30" t="s">
         <v>255</v>
       </c>
@@ -10118,7 +10155,7 @@
       </c>
       <c r="I240" s="32"/>
     </row>
-    <row r="241" spans="1:9" ht="30">
+    <row r="241" spans="1:9">
       <c r="A241" s="30" t="s">
         <v>264</v>
       </c>
@@ -10143,7 +10180,7 @@
       </c>
       <c r="I241" s="32"/>
     </row>
-    <row r="242" spans="1:9" ht="30">
+    <row r="242" spans="1:9">
       <c r="A242" s="30" t="s">
         <v>265</v>
       </c>
@@ -10218,7 +10255,7 @@
       </c>
       <c r="I244" s="32"/>
     </row>
-    <row r="245" spans="1:9" ht="105">
+    <row r="245" spans="1:9" ht="90">
       <c r="A245" s="30" t="s">
         <v>268</v>
       </c>
@@ -10243,7 +10280,7 @@
       </c>
       <c r="I245" s="32"/>
     </row>
-    <row r="246" spans="1:9" ht="45">
+    <row r="246" spans="1:9" ht="30">
       <c r="A246" s="30" t="s">
         <v>269</v>
       </c>
@@ -10270,7 +10307,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="247" spans="1:9" ht="105">
+    <row r="247" spans="1:9" ht="90">
       <c r="A247" s="30" t="s">
         <v>270</v>
       </c>
@@ -10395,7 +10432,7 @@
       </c>
       <c r="I251" s="32"/>
     </row>
-    <row r="252" spans="1:9" ht="30">
+    <row r="252" spans="1:9">
       <c r="A252" s="30" t="s">
         <v>275</v>
       </c>
@@ -10470,7 +10507,7 @@
       </c>
       <c r="I254" s="32"/>
     </row>
-    <row r="255" spans="1:9" ht="30">
+    <row r="255" spans="1:9">
       <c r="A255" s="30" t="s">
         <v>278</v>
       </c>
@@ -10495,7 +10532,7 @@
       </c>
       <c r="I255" s="32"/>
     </row>
-    <row r="256" spans="1:9" ht="30">
+    <row r="256" spans="1:9">
       <c r="A256" s="30" t="s">
         <v>279</v>
       </c>
@@ -10620,7 +10657,7 @@
       </c>
       <c r="I260" s="32"/>
     </row>
-    <row r="261" spans="1:9" ht="165">
+    <row r="261" spans="1:9" ht="135">
       <c r="A261" s="30" t="s">
         <v>284</v>
       </c>
@@ -10645,7 +10682,7 @@
       </c>
       <c r="I261" s="32"/>
     </row>
-    <row r="262" spans="1:9" ht="30">
+    <row r="262" spans="1:9">
       <c r="A262" s="30" t="s">
         <v>285</v>
       </c>
@@ -10670,7 +10707,7 @@
       </c>
       <c r="I262" s="32"/>
     </row>
-    <row r="263" spans="1:9" ht="45">
+    <row r="263" spans="1:9" ht="30">
       <c r="A263" s="30" t="s">
         <v>286</v>
       </c>
@@ -10697,7 +10734,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="264" spans="1:9" ht="105">
+    <row r="264" spans="1:9" ht="90">
       <c r="A264" s="30" t="s">
         <v>287</v>
       </c>
@@ -10747,7 +10784,7 @@
       </c>
       <c r="I265" s="32"/>
     </row>
-    <row r="266" spans="1:9" ht="75">
+    <row r="266" spans="1:9" ht="60">
       <c r="A266" s="30" t="s">
         <v>289</v>
       </c>
@@ -10847,7 +10884,7 @@
       </c>
       <c r="I269" s="32"/>
     </row>
-    <row r="270" spans="1:9" ht="45">
+    <row r="270" spans="1:9" ht="30">
       <c r="A270" s="30" t="s">
         <v>293</v>
       </c>
@@ -10872,7 +10909,7 @@
       </c>
       <c r="I270" s="32"/>
     </row>
-    <row r="271" spans="1:9" ht="30">
+    <row r="271" spans="1:9">
       <c r="A271" s="30" t="s">
         <v>294</v>
       </c>
@@ -10997,7 +11034,7 @@
       </c>
       <c r="I275" s="32"/>
     </row>
-    <row r="276" spans="1:9" ht="90">
+    <row r="276" spans="1:9" ht="75">
       <c r="A276" s="30" t="s">
         <v>299</v>
       </c>
@@ -11022,7 +11059,7 @@
       </c>
       <c r="I276" s="32"/>
     </row>
-    <row r="277" spans="1:9" ht="165">
+    <row r="277" spans="1:9" ht="150">
       <c r="A277" s="30" t="s">
         <v>300</v>
       </c>
@@ -11097,7 +11134,7 @@
       </c>
       <c r="I279" s="32"/>
     </row>
-    <row r="280" spans="1:9" ht="90">
+    <row r="280" spans="1:9" ht="75">
       <c r="A280" s="30" t="s">
         <v>303</v>
       </c>
@@ -11122,7 +11159,7 @@
       </c>
       <c r="I280" s="32"/>
     </row>
-    <row r="281" spans="1:9" ht="45">
+    <row r="281" spans="1:9" ht="30">
       <c r="A281" s="30" t="s">
         <v>304</v>
       </c>
@@ -11147,7 +11184,7 @@
       </c>
       <c r="I281" s="32"/>
     </row>
-    <row r="282" spans="1:9" ht="75">
+    <row r="282" spans="1:9" ht="60">
       <c r="A282" s="30" t="s">
         <v>305</v>
       </c>
@@ -11299,7 +11336,7 @@
       </c>
       <c r="I287" s="32"/>
     </row>
-    <row r="288" spans="1:9" ht="30">
+    <row r="288" spans="1:9">
       <c r="A288" s="30" t="s">
         <v>311</v>
       </c>
@@ -11349,7 +11386,7 @@
       </c>
       <c r="I289" s="32"/>
     </row>
-    <row r="290" spans="1:9" ht="45">
+    <row r="290" spans="1:9" ht="30">
       <c r="A290" s="30" t="s">
         <v>313</v>
       </c>
@@ -11399,7 +11436,7 @@
       </c>
       <c r="I291" s="32"/>
     </row>
-    <row r="292" spans="1:9" ht="75">
+    <row r="292" spans="1:9" ht="60">
       <c r="A292" s="30" t="s">
         <v>315</v>
       </c>
@@ -11424,7 +11461,7 @@
       </c>
       <c r="I292" s="32"/>
     </row>
-    <row r="293" spans="1:9" ht="165">
+    <row r="293" spans="1:9" ht="135">
       <c r="A293" s="30" t="s">
         <v>316</v>
       </c>
@@ -11449,7 +11486,7 @@
       </c>
       <c r="I293" s="32"/>
     </row>
-    <row r="294" spans="1:9" ht="45">
+    <row r="294" spans="1:9" ht="30">
       <c r="A294" s="30" t="s">
         <v>317</v>
       </c>
@@ -11474,7 +11511,7 @@
       </c>
       <c r="I294" s="32"/>
     </row>
-    <row r="295" spans="1:9" ht="30">
+    <row r="295" spans="1:9">
       <c r="A295" s="30" t="s">
         <v>318</v>
       </c>
@@ -11499,7 +11536,7 @@
       </c>
       <c r="I295" s="32"/>
     </row>
-    <row r="296" spans="1:9" ht="90">
+    <row r="296" spans="1:9" ht="75">
       <c r="A296" s="30" t="s">
         <v>319</v>
       </c>
@@ -11574,7 +11611,7 @@
       </c>
       <c r="I298" s="32"/>
     </row>
-    <row r="299" spans="1:9" ht="60">
+    <row r="299" spans="1:9" ht="45">
       <c r="A299" s="30" t="s">
         <v>322</v>
       </c>
@@ -11599,7 +11636,7 @@
       </c>
       <c r="I299" s="32"/>
     </row>
-    <row r="300" spans="1:9" ht="75">
+    <row r="300" spans="1:9" ht="60">
       <c r="A300" s="30" t="s">
         <v>323</v>
       </c>
@@ -11651,7 +11688,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="302" spans="1:9" ht="75">
+    <row r="302" spans="1:9" ht="60">
       <c r="A302" s="30" t="s">
         <v>325</v>
       </c>
@@ -11676,7 +11713,7 @@
       </c>
       <c r="I302" s="32"/>
     </row>
-    <row r="303" spans="1:9" ht="75">
+    <row r="303" spans="1:9" ht="60">
       <c r="A303" s="30" t="s">
         <v>326</v>
       </c>
@@ -11703,7 +11740,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="304" spans="1:9" ht="90">
+    <row r="304" spans="1:9" ht="75">
       <c r="A304" s="30" t="s">
         <v>327</v>
       </c>
@@ -11730,7 +11767,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="305" spans="1:9" ht="75">
+    <row r="305" spans="1:9" ht="45">
       <c r="A305" s="30" t="s">
         <v>328</v>
       </c>
@@ -11755,7 +11792,7 @@
       </c>
       <c r="I305" s="32"/>
     </row>
-    <row r="306" spans="1:9" ht="105">
+    <row r="306" spans="1:9" ht="90">
       <c r="A306" s="30" t="s">
         <v>329</v>
       </c>
@@ -11780,7 +11817,7 @@
       </c>
       <c r="I306" s="32"/>
     </row>
-    <row r="307" spans="1:9" ht="150">
+    <row r="307" spans="1:9" ht="135">
       <c r="A307" s="30" t="s">
         <v>763</v>
       </c>
@@ -11807,7 +11844,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="308" spans="1:9" ht="150">
+    <row r="308" spans="1:9" ht="135">
       <c r="A308" s="30" t="s">
         <v>764</v>
       </c>
@@ -11834,7 +11871,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="309" spans="1:9" ht="150">
+    <row r="309" spans="1:9" ht="120">
       <c r="A309" s="30" t="s">
         <v>330</v>
       </c>
@@ -11884,7 +11921,7 @@
       </c>
       <c r="I310" s="32"/>
     </row>
-    <row r="311" spans="1:9" ht="75">
+    <row r="311" spans="1:9" ht="60">
       <c r="A311" s="30" t="s">
         <v>332</v>
       </c>
@@ -11909,7 +11946,7 @@
       </c>
       <c r="I311" s="32"/>
     </row>
-    <row r="312" spans="1:9" ht="120">
+    <row r="312" spans="1:9" ht="90">
       <c r="A312" s="30" t="s">
         <v>333</v>
       </c>
@@ -11934,7 +11971,7 @@
       </c>
       <c r="I312" s="32"/>
     </row>
-    <row r="313" spans="1:9" ht="120">
+    <row r="313" spans="1:9" ht="90">
       <c r="A313" s="30" t="s">
         <v>334</v>
       </c>
@@ -11986,7 +12023,7 @@
       </c>
       <c r="I314" s="32"/>
     </row>
-    <row r="315" spans="1:9" ht="90">
+    <row r="315" spans="1:9" ht="75">
       <c r="A315" s="30" t="s">
         <v>336</v>
       </c>
@@ -12011,7 +12048,7 @@
       </c>
       <c r="I315" s="32"/>
     </row>
-    <row r="316" spans="1:9" ht="105">
+    <row r="316" spans="1:9" ht="90">
       <c r="A316" s="30" t="s">
         <v>337</v>
       </c>
@@ -12038,7 +12075,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="317" spans="1:9" ht="90">
+    <row r="317" spans="1:9" ht="75">
       <c r="A317" s="30" t="s">
         <v>338</v>
       </c>
@@ -12065,7 +12102,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="318" spans="1:9" ht="90">
+    <row r="318" spans="1:9" ht="75">
       <c r="A318" s="30" t="s">
         <v>339</v>
       </c>
@@ -12265,7 +12302,7 @@
       </c>
       <c r="I325" s="32"/>
     </row>
-    <row r="326" spans="1:9" ht="45">
+    <row r="326" spans="1:9" ht="30">
       <c r="A326" s="30" t="s">
         <v>347</v>
       </c>
@@ -12290,7 +12327,7 @@
       </c>
       <c r="I326" s="32"/>
     </row>
-    <row r="327" spans="1:9" ht="45">
+    <row r="327" spans="1:9" ht="30">
       <c r="A327" s="30" t="s">
         <v>348</v>
       </c>
@@ -12315,7 +12352,7 @@
       </c>
       <c r="I327" s="32"/>
     </row>
-    <row r="328" spans="1:9" ht="225">
+    <row r="328" spans="1:9" ht="195">
       <c r="A328" s="30" t="s">
         <v>349</v>
       </c>
@@ -12415,7 +12452,7 @@
       </c>
       <c r="I331" s="32"/>
     </row>
-    <row r="332" spans="1:9" ht="30">
+    <row r="332" spans="1:9">
       <c r="A332" s="30" t="s">
         <v>353</v>
       </c>
@@ -12465,7 +12502,7 @@
       </c>
       <c r="I333" s="32"/>
     </row>
-    <row r="334" spans="1:9" ht="30">
+    <row r="334" spans="1:9">
       <c r="A334" s="30" t="s">
         <v>355</v>
       </c>
@@ -12540,7 +12577,7 @@
       </c>
       <c r="I336" s="32"/>
     </row>
-    <row r="337" spans="1:9" ht="150">
+    <row r="337" spans="1:9" ht="135">
       <c r="A337" s="30" t="s">
         <v>358</v>
       </c>
@@ -12565,7 +12602,7 @@
       </c>
       <c r="I337" s="32"/>
     </row>
-    <row r="338" spans="1:9" ht="45">
+    <row r="338" spans="1:9" ht="30">
       <c r="A338" s="30" t="s">
         <v>359</v>
       </c>
@@ -12719,7 +12756,7 @@
       </c>
       <c r="I343" s="32"/>
     </row>
-    <row r="344" spans="1:9" ht="45">
+    <row r="344" spans="1:9" ht="30">
       <c r="A344" s="30" t="s">
         <v>365</v>
       </c>
@@ -12827,7 +12864,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="348" spans="1:9" ht="45">
+    <row r="348" spans="1:9" ht="30">
       <c r="A348" s="30" t="s">
         <v>369</v>
       </c>
@@ -13051,7 +13088,7 @@
       </c>
       <c r="I355" s="32"/>
     </row>
-    <row r="356" spans="1:9" ht="45">
+    <row r="356" spans="1:9" ht="30">
       <c r="A356" s="30" t="s">
         <v>373</v>
       </c>
@@ -13078,7 +13115,7 @@
       </c>
       <c r="I356" s="32"/>
     </row>
-    <row r="357" spans="1:9" ht="45">
+    <row r="357" spans="1:9" ht="30">
       <c r="A357" s="30" t="s">
         <v>374</v>
       </c>
@@ -13213,7 +13250,7 @@
       </c>
       <c r="I361" s="32"/>
     </row>
-    <row r="362" spans="1:9" ht="45">
+    <row r="362" spans="1:9" ht="30">
       <c r="A362" s="30" t="s">
         <v>834</v>
       </c>
@@ -13240,7 +13277,7 @@
       </c>
       <c r="I362" s="32"/>
     </row>
-    <row r="363" spans="1:9" ht="45">
+    <row r="363" spans="1:9" ht="30">
       <c r="A363" s="30" t="s">
         <v>835</v>
       </c>
@@ -13267,7 +13304,7 @@
       </c>
       <c r="I363" s="32"/>
     </row>
-    <row r="364" spans="1:9" ht="75">
+    <row r="364" spans="1:9" ht="60">
       <c r="A364" s="30" t="s">
         <v>377</v>
       </c>
@@ -13296,7 +13333,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="365" spans="1:9" ht="75">
+    <row r="365" spans="1:9" ht="60">
       <c r="A365" s="30" t="s">
         <v>378</v>
       </c>
@@ -13325,7 +13362,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="366" spans="1:9" ht="75">
+    <row r="366" spans="1:9" ht="60">
       <c r="A366" s="30" t="s">
         <v>379</v>
       </c>
@@ -13379,7 +13416,7 @@
       </c>
       <c r="I367" s="32"/>
     </row>
-    <row r="368" spans="1:9" ht="75">
+    <row r="368" spans="1:9" ht="60">
       <c r="A368" s="30" t="s">
         <v>848</v>
       </c>
@@ -13406,7 +13443,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="369" spans="1:9" ht="75">
+    <row r="369" spans="1:9" ht="60">
       <c r="A369" s="30" t="s">
         <v>849</v>
       </c>
@@ -13458,7 +13495,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="371" spans="1:9" ht="75">
+    <row r="371" spans="1:9" ht="60">
       <c r="A371" s="30" t="s">
         <v>857</v>
       </c>
@@ -13483,7 +13520,7 @@
       </c>
       <c r="I371" s="32"/>
     </row>
-    <row r="372" spans="1:9" ht="60">
+    <row r="372" spans="1:9" ht="45">
       <c r="A372" s="30" t="s">
         <v>381</v>
       </c>
@@ -13512,7 +13549,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="373" spans="1:9" ht="75">
+    <row r="373" spans="1:9" ht="60">
       <c r="A373" s="30" t="s">
         <v>382</v>
       </c>
@@ -13541,7 +13578,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="374" spans="1:9" ht="105">
+    <row r="374" spans="1:9" ht="90">
       <c r="A374" s="30" t="s">
         <v>383</v>
       </c>
@@ -13570,7 +13607,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="375" spans="1:9" ht="105">
+    <row r="375" spans="1:9" ht="90">
       <c r="A375" s="30" t="s">
         <v>384</v>
       </c>
@@ -13599,7 +13636,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="376" spans="1:9" ht="90">
+    <row r="376" spans="1:9" ht="75">
       <c r="A376" s="30" t="s">
         <v>385</v>
       </c>
@@ -13790,7 +13827,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B19:B147 B149:B351 B378:B380 B356:B359 B364:B367 B372:B377" numberStoredAsText="1"/>
+    <ignoredError sqref="B19:B355 B378:B380 B356:B371 B372:B377 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
[MS-OFFICIALFILE] Update RS according to v20181001 document.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-OFFICIALFILE/MS-OFFICIALFILE_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-OFFICIALFILE/MS-OFFICIALFILE_RequirementSpecification.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SHAREPOINT\SharePoint\Docs\MS-OFFICIALFILE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Works\Protocol team\Test Suites\20200429 mapi&amp;SharePoint upgrade\SharePoint\Docs\MS-OFFICIALFILE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928928CF-EFBF-43FB-A186-DFF1F9B6D85C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -25,8 +26,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="tmpC0A3" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="tmpC0A3" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\v-xuesow\AppData\Local\Temp\tmpC0A3.tmp" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -1570,12 +1571,6 @@
     <t>[In Common Message Syntax] This section contains common definitions that are used by this protocol.</t>
   </si>
   <si>
-    <t>[In Common Message Syntax] The syntax of the definitions uses XML schema, as specified in [XMLSCHEMA1] and [XMLSCHEMA2], [and WSDL, as specified in [WSDL] ].</t>
-  </si>
-  <si>
-    <t>[In Common Message Syntax] The syntax of the definitions uses [XML schema, as specified in [XMLSCHEMA1] and [XMLSCHEMA2], and] WSDL, as specified in [WSDL].</t>
-  </si>
-  <si>
     <t>[In Namespaces] This specification defines and references various XML namespaces using the mechanisms specified in [XMLNS].</t>
   </si>
   <si>
@@ -1598,9 +1593,6 @@
   </si>
   <si>
     <t>[In Namespaces] The prefix "wsdl" is used for namespace URI "http://schemas.xmlsoap.org/wsdl/", which refers to "[WSDL]".</t>
-  </si>
-  <si>
-    <t>[In Namespaces] The prefix "xs" is used for namespace URI "http://www.w3.org/2001/XMLSchema", which refers to [XMLSCHEMA1] and [XMLSCHEMA2].</t>
   </si>
   <si>
     <t>[In Complex Types] The following table summarizes the set of common XML schema complex type definitions defined by this specification.</t>
@@ -3053,10 +3045,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MS-OFFICIALFILE_R204</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3182,13 +3170,29 @@
   </si>
   <si>
     <t>[In SubmitFile] [The protocol client sends a SubmitFileSoapIn request WSDL message, and the protocol server MUST respond with a SubmitFileSoapOut response WSDL message, as follows:] [If the protocol server determines that the storage location determined by the rules has required properties that are not present in the properties element: 1. If the protocol server determines that the name of the user specified in the userName element is invalid using an implementation-specific validation algorithm, then the protocol server MUST set the ResultCode element to InvalidUser and return.] 2. Otherwise, the protocol server MUST set[the ResultCode element to MoreInformation and] the ResultUrl element to an implementation-specific URL to enter more information about the submission.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Common Message Syntax] The syntax of the definitions uses XML schema, as specified in [XMLSCHEMA1/2] and [XMLSCHEMA2/2], [and WSDL, as specified in [WSDL] ].</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Common Message Syntax] The syntax of the definitions uses [XML schema, as specified in [XMLSCHEMA1/2] and [XMLSCHEMA2/2], and] WSDL, as specified in [WSDL].</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Namespaces] The prefix "xs" is used for namespace URI "http://www.w3.org/2001/XMLSchema", which refers to [XMLSCHEMA1/2] and [XMLSCHEMA2/2].</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="177" formatCode="0.0.0"/>
@@ -3455,21 +3459,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3493,6 +3482,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4054,34 +4058,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I381" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I381"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I381" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I381" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -4090,12 +4094,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
-  <autoFilter ref="A12:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4421,7 +4425,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L383"/>
   <sheetViews>
@@ -4444,7 +4448,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>26</v>
@@ -4454,7 +4458,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -4468,138 +4472,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>846</v>
+        <v>875</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="F3" s="12">
-        <v>42566</v>
+        <v>43374</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -4612,12 +4616,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4630,12 +4634,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -4648,12 +4652,12 @@
       <c r="C14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -4666,60 +4670,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -4802,7 +4806,7 @@
         <v>17</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -4963,7 +4967,7 @@
         <v>369</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>440</v>
+        <v>876</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22" t="s">
@@ -4988,7 +4992,7 @@
         <v>369</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>441</v>
+        <v>877</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22" t="s">
@@ -5013,7 +5017,7 @@
         <v>370</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22" t="s">
@@ -5038,7 +5042,7 @@
         <v>370</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22" t="s">
@@ -5063,7 +5067,7 @@
         <v>370</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22" t="s">
@@ -5088,7 +5092,7 @@
         <v>370</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22" t="s">
@@ -5113,7 +5117,7 @@
         <v>370</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="29" t="s">
@@ -5138,7 +5142,7 @@
         <v>370</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="29" t="s">
@@ -5163,7 +5167,7 @@
         <v>370</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="29" t="s">
@@ -5188,7 +5192,7 @@
         <v>370</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29" t="s">
@@ -5212,8 +5216,8 @@
       <c r="B38" s="30" t="s">
         <v>370</v>
       </c>
-      <c r="C38" s="31" t="s">
-        <v>450</v>
+      <c r="C38" s="20" t="s">
+        <v>878</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="29" t="s">
@@ -5238,7 +5242,7 @@
         <v>371</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="29" t="s">
@@ -5263,7 +5267,7 @@
         <v>371</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D40" s="29"/>
       <c r="E40" s="29" t="s">
@@ -5288,7 +5292,7 @@
         <v>371</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D41" s="29"/>
       <c r="E41" s="29" t="s">
@@ -5313,7 +5317,7 @@
         <v>371</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D42" s="29"/>
       <c r="E42" s="29" t="s">
@@ -5338,7 +5342,7 @@
         <v>371</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="29" t="s">
@@ -5363,7 +5367,7 @@
         <v>371</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D44" s="29"/>
       <c r="E44" s="29" t="s">
@@ -5388,7 +5392,7 @@
         <v>371</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29" t="s">
@@ -5413,7 +5417,7 @@
         <v>32</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="29" t="s">
@@ -5438,7 +5442,7 @@
         <v>32</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="29" t="s">
@@ -5463,7 +5467,7 @@
         <v>32</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D48" s="29"/>
       <c r="E48" s="29" t="s">
@@ -5480,7 +5484,7 @@
       </c>
       <c r="I48" s="31"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="29" t="s">
         <v>73</v>
       </c>
@@ -5488,7 +5492,7 @@
         <v>372</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D49" s="29"/>
       <c r="E49" s="29" t="s">
@@ -5513,7 +5517,7 @@
         <v>372</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D50" s="29"/>
       <c r="E50" s="29" t="s">
@@ -5538,7 +5542,7 @@
         <v>372</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D51" s="29"/>
       <c r="E51" s="29" t="s">
@@ -5563,7 +5567,7 @@
         <v>373</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D52" s="29"/>
       <c r="E52" s="29" t="s">
@@ -5588,7 +5592,7 @@
         <v>373</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D53" s="29"/>
       <c r="E53" s="29" t="s">
@@ -5613,7 +5617,7 @@
         <v>373</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D54" s="29"/>
       <c r="E54" s="29" t="s">
@@ -5638,7 +5642,7 @@
         <v>373</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D55" s="29"/>
       <c r="E55" s="29" t="s">
@@ -5663,7 +5667,7 @@
         <v>373</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D56" s="29"/>
       <c r="E56" s="29" t="s">
@@ -5688,7 +5692,7 @@
         <v>373</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D57" s="29"/>
       <c r="E57" s="29" t="s">
@@ -5713,7 +5717,7 @@
         <v>373</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D58" s="29"/>
       <c r="E58" s="29" t="s">
@@ -5738,7 +5742,7 @@
         <v>373</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D59" s="29"/>
       <c r="E59" s="29" t="s">
@@ -5763,7 +5767,7 @@
         <v>373</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D60" s="29"/>
       <c r="E60" s="29" t="s">
@@ -5788,7 +5792,7 @@
         <v>373</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D61" s="29"/>
       <c r="E61" s="29" t="s">
@@ -5813,7 +5817,7 @@
         <v>373</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D62" s="29"/>
       <c r="E62" s="29" t="s">
@@ -5830,7 +5834,7 @@
       </c>
       <c r="I62" s="31"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="29" t="s">
         <v>87</v>
       </c>
@@ -5838,7 +5842,7 @@
         <v>373</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D63" s="29"/>
       <c r="E63" s="29" t="s">
@@ -5863,7 +5867,7 @@
         <v>373</v>
       </c>
       <c r="C64" s="31" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D64" s="29"/>
       <c r="E64" s="29" t="s">
@@ -5888,7 +5892,7 @@
         <v>373</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D65" s="29"/>
       <c r="E65" s="29" t="s">
@@ -5913,7 +5917,7 @@
         <v>373</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D66" s="29"/>
       <c r="E66" s="29" t="s">
@@ -5938,7 +5942,7 @@
         <v>373</v>
       </c>
       <c r="C67" s="31" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D67" s="29"/>
       <c r="E67" s="29" t="s">
@@ -5963,7 +5967,7 @@
         <v>373</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="D68" s="29"/>
       <c r="E68" s="29" t="s">
@@ -5988,7 +5992,7 @@
         <v>373</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="29" t="s">
@@ -6013,7 +6017,7 @@
         <v>373</v>
       </c>
       <c r="C70" s="31" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="29" t="s">
@@ -6038,7 +6042,7 @@
         <v>373</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="D71" s="29"/>
       <c r="E71" s="29" t="s">
@@ -6063,7 +6067,7 @@
         <v>373</v>
       </c>
       <c r="C72" s="31" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D72" s="29"/>
       <c r="E72" s="29" t="s">
@@ -6088,7 +6092,7 @@
         <v>373</v>
       </c>
       <c r="C73" s="31" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D73" s="29"/>
       <c r="E73" s="29" t="s">
@@ -6113,7 +6117,7 @@
         <v>373</v>
       </c>
       <c r="C74" s="31" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D74" s="29"/>
       <c r="E74" s="29" t="s">
@@ -6138,7 +6142,7 @@
         <v>373</v>
       </c>
       <c r="C75" s="31" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D75" s="29"/>
       <c r="E75" s="29" t="s">
@@ -6163,7 +6167,7 @@
         <v>373</v>
       </c>
       <c r="C76" s="31" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D76" s="29"/>
       <c r="E76" s="29" t="s">
@@ -6188,7 +6192,7 @@
         <v>373</v>
       </c>
       <c r="C77" s="31" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D77" s="29"/>
       <c r="E77" s="29" t="s">
@@ -6213,7 +6217,7 @@
         <v>374</v>
       </c>
       <c r="C78" s="31" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D78" s="29"/>
       <c r="E78" s="29" t="s">
@@ -6238,7 +6242,7 @@
         <v>374</v>
       </c>
       <c r="C79" s="31" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="D79" s="29"/>
       <c r="E79" s="29" t="s">
@@ -6263,7 +6267,7 @@
         <v>374</v>
       </c>
       <c r="C80" s="31" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D80" s="29"/>
       <c r="E80" s="29" t="s">
@@ -6288,7 +6292,7 @@
         <v>374</v>
       </c>
       <c r="C81" s="31" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D81" s="29"/>
       <c r="E81" s="29" t="s">
@@ -6313,7 +6317,7 @@
         <v>374</v>
       </c>
       <c r="C82" s="31" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D82" s="29"/>
       <c r="E82" s="29" t="s">
@@ -6338,7 +6342,7 @@
         <v>374</v>
       </c>
       <c r="C83" s="31" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D83" s="29"/>
       <c r="E83" s="29" t="s">
@@ -6363,7 +6367,7 @@
         <v>374</v>
       </c>
       <c r="C84" s="31" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D84" s="29"/>
       <c r="E84" s="29" t="s">
@@ -6388,7 +6392,7 @@
         <v>374</v>
       </c>
       <c r="C85" s="31" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D85" s="29"/>
       <c r="E85" s="29" t="s">
@@ -6413,7 +6417,7 @@
         <v>374</v>
       </c>
       <c r="C86" s="31" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D86" s="29"/>
       <c r="E86" s="29" t="s">
@@ -6438,7 +6442,7 @@
         <v>374</v>
       </c>
       <c r="C87" s="31" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D87" s="29"/>
       <c r="E87" s="29" t="s">
@@ -6463,7 +6467,7 @@
         <v>374</v>
       </c>
       <c r="C88" s="31" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D88" s="29"/>
       <c r="E88" s="29" t="s">
@@ -6488,7 +6492,7 @@
         <v>374</v>
       </c>
       <c r="C89" s="31" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D89" s="29"/>
       <c r="E89" s="29" t="s">
@@ -6504,7 +6508,7 @@
         <v>17</v>
       </c>
       <c r="I89" s="31" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -6515,7 +6519,7 @@
         <v>374</v>
       </c>
       <c r="C90" s="31" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D90" s="29"/>
       <c r="E90" s="29" t="s">
@@ -6540,7 +6544,7 @@
         <v>375</v>
       </c>
       <c r="C91" s="31" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D91" s="29"/>
       <c r="E91" s="29" t="s">
@@ -6565,7 +6569,7 @@
         <v>375</v>
       </c>
       <c r="C92" s="31" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D92" s="29"/>
       <c r="E92" s="29" t="s">
@@ -6590,7 +6594,7 @@
         <v>375</v>
       </c>
       <c r="C93" s="31" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D93" s="29"/>
       <c r="E93" s="29" t="s">
@@ -6615,7 +6619,7 @@
         <v>375</v>
       </c>
       <c r="C94" s="31" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D94" s="29"/>
       <c r="E94" s="29" t="s">
@@ -6640,7 +6644,7 @@
         <v>375</v>
       </c>
       <c r="C95" s="31" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="D95" s="29"/>
       <c r="E95" s="29" t="s">
@@ -6665,7 +6669,7 @@
         <v>375</v>
       </c>
       <c r="C96" s="31" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="D96" s="29"/>
       <c r="E96" s="29" t="s">
@@ -6690,7 +6694,7 @@
         <v>376</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="D97" s="29"/>
       <c r="E97" s="29" t="s">
@@ -6715,7 +6719,7 @@
         <v>376</v>
       </c>
       <c r="C98" s="31" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D98" s="29"/>
       <c r="E98" s="29" t="s">
@@ -6740,7 +6744,7 @@
         <v>376</v>
       </c>
       <c r="C99" s="31" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D99" s="29"/>
       <c r="E99" s="29" t="s">
@@ -6765,7 +6769,7 @@
         <v>376</v>
       </c>
       <c r="C100" s="31" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="D100" s="29"/>
       <c r="E100" s="29" t="s">
@@ -6790,7 +6794,7 @@
         <v>377</v>
       </c>
       <c r="C101" s="31" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D101" s="29"/>
       <c r="E101" s="29" t="s">
@@ -6815,7 +6819,7 @@
         <v>377</v>
       </c>
       <c r="C102" s="31" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="D102" s="29"/>
       <c r="E102" s="29" t="s">
@@ -6840,7 +6844,7 @@
         <v>377</v>
       </c>
       <c r="C103" s="31" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D103" s="29"/>
       <c r="E103" s="29" t="s">
@@ -6865,7 +6869,7 @@
         <v>377</v>
       </c>
       <c r="C104" s="31" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D104" s="29"/>
       <c r="E104" s="29" t="s">
@@ -6890,7 +6894,7 @@
         <v>377</v>
       </c>
       <c r="C105" s="31" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D105" s="29"/>
       <c r="E105" s="29" t="s">
@@ -6915,7 +6919,7 @@
         <v>377</v>
       </c>
       <c r="C106" s="31" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D106" s="29"/>
       <c r="E106" s="29" t="s">
@@ -6940,7 +6944,7 @@
         <v>378</v>
       </c>
       <c r="C107" s="31" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="D107" s="29"/>
       <c r="E107" s="29" t="s">
@@ -6965,7 +6969,7 @@
         <v>378</v>
       </c>
       <c r="C108" s="31" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D108" s="29"/>
       <c r="E108" s="29" t="s">
@@ -6990,7 +6994,7 @@
         <v>378</v>
       </c>
       <c r="C109" s="31" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D109" s="29"/>
       <c r="E109" s="29" t="s">
@@ -7007,7 +7011,7 @@
       </c>
       <c r="I109" s="31"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="29" t="s">
         <v>134</v>
       </c>
@@ -7015,7 +7019,7 @@
         <v>378</v>
       </c>
       <c r="C110" s="31" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="D110" s="29"/>
       <c r="E110" s="29" t="s">
@@ -7040,7 +7044,7 @@
         <v>378</v>
       </c>
       <c r="C111" s="31" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D111" s="29"/>
       <c r="E111" s="29" t="s">
@@ -7065,7 +7069,7 @@
         <v>378</v>
       </c>
       <c r="C112" s="31" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D112" s="29"/>
       <c r="E112" s="29" t="s">
@@ -7090,7 +7094,7 @@
         <v>378</v>
       </c>
       <c r="C113" s="31" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D113" s="29"/>
       <c r="E113" s="29" t="s">
@@ -7115,7 +7119,7 @@
         <v>378</v>
       </c>
       <c r="C114" s="31" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D114" s="29"/>
       <c r="E114" s="29" t="s">
@@ -7140,7 +7144,7 @@
         <v>378</v>
       </c>
       <c r="C115" s="31" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D115" s="29"/>
       <c r="E115" s="29" t="s">
@@ -7165,7 +7169,7 @@
         <v>378</v>
       </c>
       <c r="C116" s="31" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D116" s="29"/>
       <c r="E116" s="29" t="s">
@@ -7190,7 +7194,7 @@
         <v>378</v>
       </c>
       <c r="C117" s="31" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D117" s="29"/>
       <c r="E117" s="29" t="s">
@@ -7215,7 +7219,7 @@
         <v>379</v>
       </c>
       <c r="C118" s="31" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D118" s="29"/>
       <c r="E118" s="29" t="s">
@@ -7240,7 +7244,7 @@
         <v>379</v>
       </c>
       <c r="C119" s="31" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D119" s="29"/>
       <c r="E119" s="29" t="s">
@@ -7265,7 +7269,7 @@
         <v>379</v>
       </c>
       <c r="C120" s="31" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="D120" s="29"/>
       <c r="E120" s="29" t="s">
@@ -7290,7 +7294,7 @@
         <v>379</v>
       </c>
       <c r="C121" s="31" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D121" s="29"/>
       <c r="E121" s="29" t="s">
@@ -7315,7 +7319,7 @@
         <v>379</v>
       </c>
       <c r="C122" s="31" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D122" s="29"/>
       <c r="E122" s="29" t="s">
@@ -7340,7 +7344,7 @@
         <v>379</v>
       </c>
       <c r="C123" s="31" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D123" s="29"/>
       <c r="E123" s="29" t="s">
@@ -7357,7 +7361,7 @@
       </c>
       <c r="I123" s="31"/>
     </row>
-    <row r="124" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="29" t="s">
         <v>148</v>
       </c>
@@ -7365,7 +7369,7 @@
         <v>379</v>
       </c>
       <c r="C124" s="31" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D124" s="29"/>
       <c r="E124" s="29" t="s">
@@ -7390,7 +7394,7 @@
         <v>379</v>
       </c>
       <c r="C125" s="31" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D125" s="29"/>
       <c r="E125" s="29" t="s">
@@ -7415,7 +7419,7 @@
         <v>379</v>
       </c>
       <c r="C126" s="31" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D126" s="29"/>
       <c r="E126" s="29" t="s">
@@ -7440,7 +7444,7 @@
         <v>379</v>
       </c>
       <c r="C127" s="31" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D127" s="29"/>
       <c r="E127" s="29" t="s">
@@ -7465,7 +7469,7 @@
         <v>379</v>
       </c>
       <c r="C128" s="31" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="29" t="s">
@@ -7490,7 +7494,7 @@
         <v>380</v>
       </c>
       <c r="C129" s="31" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D129" s="29"/>
       <c r="E129" s="29" t="s">
@@ -7515,7 +7519,7 @@
         <v>380</v>
       </c>
       <c r="C130" s="31" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="D130" s="29"/>
       <c r="E130" s="29" t="s">
@@ -7540,7 +7544,7 @@
         <v>380</v>
       </c>
       <c r="C131" s="31" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D131" s="29"/>
       <c r="E131" s="29" t="s">
@@ -7565,7 +7569,7 @@
         <v>380</v>
       </c>
       <c r="C132" s="31" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="D132" s="29"/>
       <c r="E132" s="29" t="s">
@@ -7590,7 +7594,7 @@
         <v>380</v>
       </c>
       <c r="C133" s="31" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="D133" s="29"/>
       <c r="E133" s="29" t="s">
@@ -7615,7 +7619,7 @@
         <v>380</v>
       </c>
       <c r="C134" s="31" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D134" s="29"/>
       <c r="E134" s="29" t="s">
@@ -7640,7 +7644,7 @@
         <v>380</v>
       </c>
       <c r="C135" s="31" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="D135" s="29"/>
       <c r="E135" s="29" t="s">
@@ -7665,7 +7669,7 @@
         <v>380</v>
       </c>
       <c r="C136" s="31" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="D136" s="29"/>
       <c r="E136" s="29" t="s">
@@ -7690,7 +7694,7 @@
         <v>380</v>
       </c>
       <c r="C137" s="31" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D137" s="29"/>
       <c r="E137" s="29" t="s">
@@ -7715,7 +7719,7 @@
         <v>380</v>
       </c>
       <c r="C138" s="31" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="D138" s="29"/>
       <c r="E138" s="29" t="s">
@@ -7740,7 +7744,7 @@
         <v>380</v>
       </c>
       <c r="C139" s="31" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="D139" s="29"/>
       <c r="E139" s="29" t="s">
@@ -7765,7 +7769,7 @@
         <v>381</v>
       </c>
       <c r="C140" s="31" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="D140" s="29"/>
       <c r="E140" s="29" t="s">
@@ -7790,7 +7794,7 @@
         <v>381</v>
       </c>
       <c r="C141" s="31" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D141" s="29"/>
       <c r="E141" s="29" t="s">
@@ -7806,7 +7810,7 @@
         <v>17</v>
       </c>
       <c r="I141" s="31" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -7817,7 +7821,7 @@
         <v>381</v>
       </c>
       <c r="C142" s="31" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D142" s="29"/>
       <c r="E142" s="29" t="s">
@@ -7833,7 +7837,7 @@
         <v>17</v>
       </c>
       <c r="I142" s="31" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -7844,7 +7848,7 @@
         <v>381</v>
       </c>
       <c r="C143" s="31" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="29" t="s">
@@ -7860,7 +7864,7 @@
         <v>17</v>
       </c>
       <c r="I143" s="31" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -7871,7 +7875,7 @@
         <v>381</v>
       </c>
       <c r="C144" s="31" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="D144" s="29"/>
       <c r="E144" s="29" t="s">
@@ -7887,10 +7891,10 @@
         <v>17</v>
       </c>
       <c r="I144" s="31" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A145" s="29" t="s">
         <v>169</v>
       </c>
@@ -7898,7 +7902,7 @@
         <v>381</v>
       </c>
       <c r="C145" s="31" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="D145" s="29"/>
       <c r="E145" s="29" t="s">
@@ -7917,13 +7921,13 @@
     </row>
     <row r="146" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="29" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="B146" s="30" t="s">
         <v>381</v>
       </c>
       <c r="C146" s="31" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D146" s="29"/>
       <c r="E146" s="29" t="s">
@@ -7942,13 +7946,13 @@
     </row>
     <row r="147" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="29" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="B147" s="30" t="s">
         <v>33</v>
       </c>
       <c r="C147" s="31" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="D147" s="29"/>
       <c r="E147" s="29" t="s">
@@ -7961,19 +7965,19 @@
         <v>15</v>
       </c>
       <c r="H147" s="29" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="I147" s="31"/>
     </row>
     <row r="148" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="29" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="B148" s="30" t="s">
         <v>33</v>
       </c>
       <c r="C148" s="31" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="D148" s="29"/>
       <c r="E148" s="29" t="s">
@@ -7998,7 +8002,7 @@
         <v>33</v>
       </c>
       <c r="C149" s="31" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D149" s="29"/>
       <c r="E149" s="29" t="s">
@@ -8023,7 +8027,7 @@
         <v>33</v>
       </c>
       <c r="C150" s="31" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="D150" s="29"/>
       <c r="E150" s="29" t="s">
@@ -8048,7 +8052,7 @@
         <v>33</v>
       </c>
       <c r="C151" s="31" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="D151" s="29"/>
       <c r="E151" s="29" t="s">
@@ -8073,7 +8077,7 @@
         <v>33</v>
       </c>
       <c r="C152" s="31" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D152" s="29"/>
       <c r="E152" s="29" t="s">
@@ -8098,7 +8102,7 @@
         <v>33</v>
       </c>
       <c r="C153" s="31" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D153" s="29"/>
       <c r="E153" s="29" t="s">
@@ -8123,7 +8127,7 @@
         <v>33</v>
       </c>
       <c r="C154" s="31" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="D154" s="29"/>
       <c r="E154" s="29" t="s">
@@ -8148,7 +8152,7 @@
         <v>33</v>
       </c>
       <c r="C155" s="31" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D155" s="29"/>
       <c r="E155" s="29" t="s">
@@ -8165,7 +8169,7 @@
       </c>
       <c r="I155" s="31"/>
     </row>
-    <row r="156" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A156" s="29" t="s">
         <v>177</v>
       </c>
@@ -8173,7 +8177,7 @@
         <v>33</v>
       </c>
       <c r="C156" s="31" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="D156" s="29"/>
       <c r="E156" s="29" t="s">
@@ -8198,7 +8202,7 @@
         <v>33</v>
       </c>
       <c r="C157" s="31" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="D157" s="29"/>
       <c r="E157" s="29" t="s">
@@ -8223,7 +8227,7 @@
         <v>33</v>
       </c>
       <c r="C158" s="31" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D158" s="29"/>
       <c r="E158" s="29" t="s">
@@ -8240,7 +8244,7 @@
       </c>
       <c r="I158" s="31"/>
     </row>
-    <row r="159" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A159" s="29" t="s">
         <v>180</v>
       </c>
@@ -8248,7 +8252,7 @@
         <v>33</v>
       </c>
       <c r="C159" s="31" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D159" s="29"/>
       <c r="E159" s="29" t="s">
@@ -8273,7 +8277,7 @@
         <v>33</v>
       </c>
       <c r="C160" s="31" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D160" s="29"/>
       <c r="E160" s="29" t="s">
@@ -8289,7 +8293,7 @@
         <v>17</v>
       </c>
       <c r="I160" s="31" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -8300,10 +8304,10 @@
         <v>33</v>
       </c>
       <c r="C161" s="31" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="D161" s="29" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="E161" s="29" t="s">
         <v>19</v>
@@ -8327,7 +8331,7 @@
         <v>33</v>
       </c>
       <c r="C162" s="31" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="D162" s="29"/>
       <c r="E162" s="29" t="s">
@@ -8352,7 +8356,7 @@
         <v>33</v>
       </c>
       <c r="C163" s="31" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D163" s="29"/>
       <c r="E163" s="29" t="s">
@@ -8377,7 +8381,7 @@
         <v>33</v>
       </c>
       <c r="C164" s="31" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="D164" s="29"/>
       <c r="E164" s="29" t="s">
@@ -8402,7 +8406,7 @@
         <v>33</v>
       </c>
       <c r="C165" s="31" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="D165" s="29"/>
       <c r="E165" s="29" t="s">
@@ -8427,7 +8431,7 @@
         <v>33</v>
       </c>
       <c r="C166" s="31" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="D166" s="29"/>
       <c r="E166" s="29" t="s">
@@ -8452,7 +8456,7 @@
         <v>33</v>
       </c>
       <c r="C167" s="31" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="D167" s="29"/>
       <c r="E167" s="29" t="s">
@@ -8477,7 +8481,7 @@
         <v>382</v>
       </c>
       <c r="C168" s="31" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="D168" s="29"/>
       <c r="E168" s="29" t="s">
@@ -8502,7 +8506,7 @@
         <v>382</v>
       </c>
       <c r="C169" s="31" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="D169" s="29"/>
       <c r="E169" s="29" t="s">
@@ -8527,7 +8531,7 @@
         <v>383</v>
       </c>
       <c r="C170" s="31" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="D170" s="29"/>
       <c r="E170" s="29" t="s">
@@ -8552,7 +8556,7 @@
         <v>383</v>
       </c>
       <c r="C171" s="31" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D171" s="29"/>
       <c r="E171" s="29" t="s">
@@ -8577,7 +8581,7 @@
         <v>383</v>
       </c>
       <c r="C172" s="31" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="D172" s="29"/>
       <c r="E172" s="29" t="s">
@@ -8602,7 +8606,7 @@
         <v>384</v>
       </c>
       <c r="C173" s="31" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D173" s="29"/>
       <c r="E173" s="29" t="s">
@@ -8627,7 +8631,7 @@
         <v>384</v>
       </c>
       <c r="C174" s="31" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="D174" s="29"/>
       <c r="E174" s="29" t="s">
@@ -8652,7 +8656,7 @@
         <v>385</v>
       </c>
       <c r="C175" s="31" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="D175" s="29"/>
       <c r="E175" s="29" t="s">
@@ -8677,7 +8681,7 @@
         <v>385</v>
       </c>
       <c r="C176" s="31" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="D176" s="29"/>
       <c r="E176" s="29" t="s">
@@ -8694,7 +8698,7 @@
       </c>
       <c r="I176" s="31"/>
     </row>
-    <row r="177" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" ht="195" x14ac:dyDescent="0.25">
       <c r="A177" s="29" t="s">
         <v>198</v>
       </c>
@@ -8702,7 +8706,7 @@
         <v>386</v>
       </c>
       <c r="C177" s="31" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="D177" s="29"/>
       <c r="E177" s="29" t="s">
@@ -8727,7 +8731,7 @@
         <v>386</v>
       </c>
       <c r="C178" s="31" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="D178" s="29"/>
       <c r="E178" s="29" t="s">
@@ -8752,7 +8756,7 @@
         <v>386</v>
       </c>
       <c r="C179" s="31" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="D179" s="29"/>
       <c r="E179" s="29" t="s">
@@ -8777,7 +8781,7 @@
         <v>386</v>
       </c>
       <c r="C180" s="31" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="D180" s="29"/>
       <c r="E180" s="29" t="s">
@@ -8802,7 +8806,7 @@
         <v>387</v>
       </c>
       <c r="C181" s="31" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D181" s="29"/>
       <c r="E181" s="29" t="s">
@@ -8827,7 +8831,7 @@
         <v>387</v>
       </c>
       <c r="C182" s="31" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="D182" s="29"/>
       <c r="E182" s="29" t="s">
@@ -8852,7 +8856,7 @@
         <v>388</v>
       </c>
       <c r="C183" s="31" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D183" s="29"/>
       <c r="E183" s="29" t="s">
@@ -8869,7 +8873,7 @@
       </c>
       <c r="I183" s="31"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="29" t="s">
         <v>205</v>
       </c>
@@ -8877,7 +8881,7 @@
         <v>389</v>
       </c>
       <c r="C184" s="31" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="D184" s="29"/>
       <c r="E184" s="29" t="s">
@@ -8902,7 +8906,7 @@
         <v>389</v>
       </c>
       <c r="C185" s="31" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="D185" s="29"/>
       <c r="E185" s="29" t="s">
@@ -8927,7 +8931,7 @@
         <v>389</v>
       </c>
       <c r="C186" s="31" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D186" s="29"/>
       <c r="E186" s="29" t="s">
@@ -8944,7 +8948,7 @@
       </c>
       <c r="I186" s="31"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A187" s="29" t="s">
         <v>208</v>
       </c>
@@ -8952,7 +8956,7 @@
         <v>389</v>
       </c>
       <c r="C187" s="31" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="D187" s="29"/>
       <c r="E187" s="29" t="s">
@@ -8977,7 +8981,7 @@
         <v>389</v>
       </c>
       <c r="C188" s="31" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="D188" s="29"/>
       <c r="E188" s="29" t="s">
@@ -9002,7 +9006,7 @@
         <v>390</v>
       </c>
       <c r="C189" s="31" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D189" s="29"/>
       <c r="E189" s="29" t="s">
@@ -9027,7 +9031,7 @@
         <v>390</v>
       </c>
       <c r="C190" s="31" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="D190" s="29"/>
       <c r="E190" s="29" t="s">
@@ -9052,7 +9056,7 @@
         <v>391</v>
       </c>
       <c r="C191" s="31" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="D191" s="29"/>
       <c r="E191" s="29" t="s">
@@ -9077,7 +9081,7 @@
         <v>391</v>
       </c>
       <c r="C192" s="31" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="D192" s="29"/>
       <c r="E192" s="29" t="s">
@@ -9102,7 +9106,7 @@
         <v>391</v>
       </c>
       <c r="C193" s="31" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D193" s="29"/>
       <c r="E193" s="29" t="s">
@@ -9127,7 +9131,7 @@
         <v>391</v>
       </c>
       <c r="C194" s="31" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="D194" s="29"/>
       <c r="E194" s="29" t="s">
@@ -9152,7 +9156,7 @@
         <v>391</v>
       </c>
       <c r="C195" s="31" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="D195" s="29"/>
       <c r="E195" s="29" t="s">
@@ -9177,7 +9181,7 @@
         <v>391</v>
       </c>
       <c r="C196" s="31" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="D196" s="29"/>
       <c r="E196" s="29" t="s">
@@ -9202,7 +9206,7 @@
         <v>391</v>
       </c>
       <c r="C197" s="31" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D197" s="29"/>
       <c r="E197" s="29" t="s">
@@ -9227,7 +9231,7 @@
         <v>391</v>
       </c>
       <c r="C198" s="31" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D198" s="29"/>
       <c r="E198" s="29" t="s">
@@ -9252,7 +9256,7 @@
         <v>391</v>
       </c>
       <c r="C199" s="31" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D199" s="29"/>
       <c r="E199" s="29" t="s">
@@ -9277,7 +9281,7 @@
         <v>391</v>
       </c>
       <c r="C200" s="31" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="D200" s="29"/>
       <c r="E200" s="29" t="s">
@@ -9302,7 +9306,7 @@
         <v>391</v>
       </c>
       <c r="C201" s="31" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="D201" s="29"/>
       <c r="E201" s="29" t="s">
@@ -9327,7 +9331,7 @@
         <v>391</v>
       </c>
       <c r="C202" s="31" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="D202" s="29"/>
       <c r="E202" s="29" t="s">
@@ -9352,7 +9356,7 @@
         <v>391</v>
       </c>
       <c r="C203" s="31" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="D203" s="29"/>
       <c r="E203" s="29" t="s">
@@ -9377,7 +9381,7 @@
         <v>392</v>
       </c>
       <c r="C204" s="31" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="D204" s="29"/>
       <c r="E204" s="29" t="s">
@@ -9402,7 +9406,7 @@
         <v>392</v>
       </c>
       <c r="C205" s="31" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="D205" s="29"/>
       <c r="E205" s="29" t="s">
@@ -9419,7 +9423,7 @@
       </c>
       <c r="I205" s="31"/>
     </row>
-    <row r="206" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A206" s="29" t="s">
         <v>227</v>
       </c>
@@ -9427,7 +9431,7 @@
         <v>392</v>
       </c>
       <c r="C206" s="31" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="D206" s="29"/>
       <c r="E206" s="29" t="s">
@@ -9452,7 +9456,7 @@
         <v>392</v>
       </c>
       <c r="C207" s="31" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="D207" s="29"/>
       <c r="E207" s="29" t="s">
@@ -9477,7 +9481,7 @@
         <v>392</v>
       </c>
       <c r="C208" s="31" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="D208" s="29"/>
       <c r="E208" s="29" t="s">
@@ -9502,7 +9506,7 @@
         <v>392</v>
       </c>
       <c r="C209" s="31" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="D209" s="29"/>
       <c r="E209" s="29" t="s">
@@ -9527,7 +9531,7 @@
         <v>392</v>
       </c>
       <c r="C210" s="31" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="D210" s="29"/>
       <c r="E210" s="29" t="s">
@@ -9552,7 +9556,7 @@
         <v>34</v>
       </c>
       <c r="C211" s="31" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="D211" s="29"/>
       <c r="E211" s="29" t="s">
@@ -9577,7 +9581,7 @@
         <v>34</v>
       </c>
       <c r="C212" s="31" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="D212" s="29"/>
       <c r="E212" s="29" t="s">
@@ -9602,7 +9606,7 @@
         <v>34</v>
       </c>
       <c r="C213" s="31" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="D213" s="29"/>
       <c r="E213" s="29" t="s">
@@ -9627,7 +9631,7 @@
         <v>34</v>
       </c>
       <c r="C214" s="31" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="D214" s="29"/>
       <c r="E214" s="29" t="s">
@@ -9652,7 +9656,7 @@
         <v>393</v>
       </c>
       <c r="C215" s="31" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D215" s="29"/>
       <c r="E215" s="29" t="s">
@@ -9677,7 +9681,7 @@
         <v>393</v>
       </c>
       <c r="C216" s="31" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="D216" s="29"/>
       <c r="E216" s="29" t="s">
@@ -9702,7 +9706,7 @@
         <v>394</v>
       </c>
       <c r="C217" s="31" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="D217" s="29"/>
       <c r="E217" s="29" t="s">
@@ -9727,7 +9731,7 @@
         <v>394</v>
       </c>
       <c r="C218" s="31" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="D218" s="29"/>
       <c r="E218" s="29" t="s">
@@ -9752,7 +9756,7 @@
         <v>394</v>
       </c>
       <c r="C219" s="31" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="D219" s="29"/>
       <c r="E219" s="29" t="s">
@@ -9777,7 +9781,7 @@
         <v>395</v>
       </c>
       <c r="C220" s="31" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D220" s="29"/>
       <c r="E220" s="29" t="s">
@@ -9802,7 +9806,7 @@
         <v>395</v>
       </c>
       <c r="C221" s="31" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="D221" s="29"/>
       <c r="E221" s="29" t="s">
@@ -9827,7 +9831,7 @@
         <v>396</v>
       </c>
       <c r="C222" s="31" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="D222" s="29"/>
       <c r="E222" s="29" t="s">
@@ -9844,7 +9848,7 @@
       </c>
       <c r="I222" s="31"/>
     </row>
-    <row r="223" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A223" s="29" t="s">
         <v>244</v>
       </c>
@@ -9852,7 +9856,7 @@
         <v>396</v>
       </c>
       <c r="C223" s="31" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="D223" s="29"/>
       <c r="E223" s="29" t="s">
@@ -9877,7 +9881,7 @@
         <v>397</v>
       </c>
       <c r="C224" s="31" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="D224" s="29"/>
       <c r="E224" s="29" t="s">
@@ -9902,7 +9906,7 @@
         <v>398</v>
       </c>
       <c r="C225" s="31" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="D225" s="29"/>
       <c r="E225" s="29" t="s">
@@ -9927,7 +9931,7 @@
         <v>398</v>
       </c>
       <c r="C226" s="31" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="D226" s="29"/>
       <c r="E226" s="29" t="s">
@@ -9952,7 +9956,7 @@
         <v>399</v>
       </c>
       <c r="C227" s="31" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D227" s="29"/>
       <c r="E227" s="29" t="s">
@@ -9977,7 +9981,7 @@
         <v>399</v>
       </c>
       <c r="C228" s="31" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="D228" s="29"/>
       <c r="E228" s="29" t="s">
@@ -10002,7 +10006,7 @@
         <v>400</v>
       </c>
       <c r="C229" s="31" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="D229" s="29"/>
       <c r="E229" s="29" t="s">
@@ -10019,7 +10023,7 @@
       </c>
       <c r="I229" s="31"/>
     </row>
-    <row r="230" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A230" s="29" t="s">
         <v>251</v>
       </c>
@@ -10027,7 +10031,7 @@
         <v>400</v>
       </c>
       <c r="C230" s="31" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="D230" s="29"/>
       <c r="E230" s="29" t="s">
@@ -10052,7 +10056,7 @@
         <v>400</v>
       </c>
       <c r="C231" s="31" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="D231" s="29"/>
       <c r="E231" s="29" t="s">
@@ -10077,7 +10081,7 @@
         <v>401</v>
       </c>
       <c r="C232" s="31" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="D232" s="29"/>
       <c r="E232" s="29" t="s">
@@ -10102,7 +10106,7 @@
         <v>401</v>
       </c>
       <c r="C233" s="31" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="D233" s="29"/>
       <c r="E233" s="29" t="s">
@@ -10127,7 +10131,7 @@
         <v>401</v>
       </c>
       <c r="C234" s="31" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="D234" s="29"/>
       <c r="E234" s="29" t="s">
@@ -10152,7 +10156,7 @@
         <v>401</v>
       </c>
       <c r="C235" s="31" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="D235" s="29"/>
       <c r="E235" s="29" t="s">
@@ -10177,7 +10181,7 @@
         <v>401</v>
       </c>
       <c r="C236" s="31" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="D236" s="29"/>
       <c r="E236" s="29" t="s">
@@ -10202,7 +10206,7 @@
         <v>401</v>
       </c>
       <c r="C237" s="31" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="D237" s="29"/>
       <c r="E237" s="29" t="s">
@@ -10227,7 +10231,7 @@
         <v>401</v>
       </c>
       <c r="C238" s="31" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="D238" s="29"/>
       <c r="E238" s="29" t="s">
@@ -10252,7 +10256,7 @@
         <v>401</v>
       </c>
       <c r="C239" s="31" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="D239" s="29"/>
       <c r="E239" s="29" t="s">
@@ -10277,7 +10281,7 @@
         <v>401</v>
       </c>
       <c r="C240" s="31" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="D240" s="29"/>
       <c r="E240" s="29" t="s">
@@ -10302,7 +10306,7 @@
         <v>401</v>
       </c>
       <c r="C241" s="31" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="D241" s="29"/>
       <c r="E241" s="29" t="s">
@@ -10327,7 +10331,7 @@
         <v>401</v>
       </c>
       <c r="C242" s="31" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="D242" s="29"/>
       <c r="E242" s="29" t="s">
@@ -10352,7 +10356,7 @@
         <v>402</v>
       </c>
       <c r="C243" s="31" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="D243" s="29"/>
       <c r="E243" s="29" t="s">
@@ -10377,7 +10381,7 @@
         <v>403</v>
       </c>
       <c r="C244" s="31" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="D244" s="29"/>
       <c r="E244" s="29" t="s">
@@ -10402,7 +10406,7 @@
         <v>403</v>
       </c>
       <c r="C245" s="31" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="D245" s="29"/>
       <c r="E245" s="29" t="s">
@@ -10427,7 +10431,7 @@
         <v>404</v>
       </c>
       <c r="C246" s="31" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="D246" s="29"/>
       <c r="E246" s="29" t="s">
@@ -10452,7 +10456,7 @@
         <v>404</v>
       </c>
       <c r="C247" s="31" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D247" s="29"/>
       <c r="E247" s="29" t="s">
@@ -10477,7 +10481,7 @@
         <v>404</v>
       </c>
       <c r="C248" s="31" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="D248" s="29"/>
       <c r="E248" s="29" t="s">
@@ -10502,7 +10506,7 @@
         <v>404</v>
       </c>
       <c r="C249" s="31" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="D249" s="29"/>
       <c r="E249" s="29" t="s">
@@ -10527,7 +10531,7 @@
         <v>405</v>
       </c>
       <c r="C250" s="31" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="D250" s="29"/>
       <c r="E250" s="29" t="s">
@@ -10552,7 +10556,7 @@
         <v>405</v>
       </c>
       <c r="C251" s="31" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="D251" s="29"/>
       <c r="E251" s="29" t="s">
@@ -10577,7 +10581,7 @@
         <v>406</v>
       </c>
       <c r="C252" s="31" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="D252" s="29"/>
       <c r="E252" s="29" t="s">
@@ -10602,7 +10606,7 @@
         <v>406</v>
       </c>
       <c r="C253" s="31" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="D253" s="29"/>
       <c r="E253" s="29" t="s">
@@ -10627,7 +10631,7 @@
         <v>406</v>
       </c>
       <c r="C254" s="31" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="D254" s="29"/>
       <c r="E254" s="29" t="s">
@@ -10652,7 +10656,7 @@
         <v>407</v>
       </c>
       <c r="C255" s="31" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="D255" s="29"/>
       <c r="E255" s="29" t="s">
@@ -10677,7 +10681,7 @@
         <v>407</v>
       </c>
       <c r="C256" s="31" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="D256" s="29"/>
       <c r="E256" s="29" t="s">
@@ -10694,7 +10698,7 @@
       </c>
       <c r="I256" s="31"/>
     </row>
-    <row r="257" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A257" s="29" t="s">
         <v>278</v>
       </c>
@@ -10702,7 +10706,7 @@
         <v>408</v>
       </c>
       <c r="C257" s="31" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="D257" s="29"/>
       <c r="E257" s="29" t="s">
@@ -10727,7 +10731,7 @@
         <v>408</v>
       </c>
       <c r="C258" s="31" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="D258" s="29"/>
       <c r="E258" s="29" t="s">
@@ -10752,7 +10756,7 @@
         <v>409</v>
       </c>
       <c r="C259" s="31" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="D259" s="29"/>
       <c r="E259" s="29" t="s">
@@ -10777,7 +10781,7 @@
         <v>409</v>
       </c>
       <c r="C260" s="31" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="D260" s="29"/>
       <c r="E260" s="29" t="s">
@@ -10802,7 +10806,7 @@
         <v>410</v>
       </c>
       <c r="C261" s="31" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="D261" s="29"/>
       <c r="E261" s="29" t="s">
@@ -10827,7 +10831,7 @@
         <v>410</v>
       </c>
       <c r="C262" s="31" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="D262" s="29"/>
       <c r="E262" s="29" t="s">
@@ -10846,13 +10850,13 @@
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" s="29" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="B263" s="30" t="s">
         <v>411</v>
       </c>
       <c r="C263" s="31" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="D263" s="29"/>
       <c r="E263" s="29" t="s">
@@ -10877,7 +10881,7 @@
         <v>411</v>
       </c>
       <c r="C264" s="31" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="D264" s="29"/>
       <c r="E264" s="29" t="s">
@@ -10902,7 +10906,7 @@
         <v>411</v>
       </c>
       <c r="C265" s="31" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="D265" s="29"/>
       <c r="E265" s="29" t="s">
@@ -10927,7 +10931,7 @@
         <v>411</v>
       </c>
       <c r="C266" s="31" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="D266" s="29"/>
       <c r="E266" s="29" t="s">
@@ -10952,7 +10956,7 @@
         <v>412</v>
       </c>
       <c r="C267" s="31" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="D267" s="29"/>
       <c r="E267" s="29" t="s">
@@ -10977,7 +10981,7 @@
         <v>412</v>
       </c>
       <c r="C268" s="31" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="D268" s="29"/>
       <c r="E268" s="29" t="s">
@@ -11002,7 +11006,7 @@
         <v>413</v>
       </c>
       <c r="C269" s="31" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="D269" s="29"/>
       <c r="E269" s="29" t="s">
@@ -11027,7 +11031,7 @@
         <v>413</v>
       </c>
       <c r="C270" s="31" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="D270" s="29"/>
       <c r="E270" s="29" t="s">
@@ -11052,7 +11056,7 @@
         <v>413</v>
       </c>
       <c r="C271" s="31" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="D271" s="29"/>
       <c r="E271" s="29" t="s">
@@ -11077,7 +11081,7 @@
         <v>414</v>
       </c>
       <c r="C272" s="31" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="D272" s="29"/>
       <c r="E272" s="29" t="s">
@@ -11102,7 +11106,7 @@
         <v>414</v>
       </c>
       <c r="C273" s="31" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="D273" s="29"/>
       <c r="E273" s="29" t="s">
@@ -11127,7 +11131,7 @@
         <v>415</v>
       </c>
       <c r="C274" s="31" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="D274" s="29"/>
       <c r="E274" s="29" t="s">
@@ -11152,7 +11156,7 @@
         <v>415</v>
       </c>
       <c r="C275" s="31" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="D275" s="29"/>
       <c r="E275" s="29" t="s">
@@ -11177,7 +11181,7 @@
         <v>416</v>
       </c>
       <c r="C276" s="31" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="D276" s="29"/>
       <c r="E276" s="29" t="s">
@@ -11194,7 +11198,7 @@
       </c>
       <c r="I276" s="31"/>
     </row>
-    <row r="277" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A277" s="29" t="s">
         <v>297</v>
       </c>
@@ -11202,7 +11206,7 @@
         <v>417</v>
       </c>
       <c r="C277" s="31" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="D277" s="29"/>
       <c r="E277" s="29" t="s">
@@ -11227,7 +11231,7 @@
         <v>417</v>
       </c>
       <c r="C278" s="31" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="D278" s="29"/>
       <c r="E278" s="29" t="s">
@@ -11252,7 +11256,7 @@
         <v>418</v>
       </c>
       <c r="C279" s="31" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="D279" s="29"/>
       <c r="E279" s="29" t="s">
@@ -11277,7 +11281,7 @@
         <v>418</v>
       </c>
       <c r="C280" s="31" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="D280" s="29"/>
       <c r="E280" s="29" t="s">
@@ -11302,7 +11306,7 @@
         <v>418</v>
       </c>
       <c r="C281" s="31" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="D281" s="29"/>
       <c r="E281" s="29" t="s">
@@ -11327,7 +11331,7 @@
         <v>418</v>
       </c>
       <c r="C282" s="31" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="D282" s="29"/>
       <c r="E282" s="29" t="s">
@@ -11343,7 +11347,7 @@
         <v>17</v>
       </c>
       <c r="I282" s="31" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="283" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -11354,7 +11358,7 @@
         <v>419</v>
       </c>
       <c r="C283" s="31" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="D283" s="29"/>
       <c r="E283" s="29" t="s">
@@ -11379,7 +11383,7 @@
         <v>419</v>
       </c>
       <c r="C284" s="31" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="D284" s="29"/>
       <c r="E284" s="29" t="s">
@@ -11404,7 +11408,7 @@
         <v>420</v>
       </c>
       <c r="C285" s="31" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="D285" s="29"/>
       <c r="E285" s="29" t="s">
@@ -11429,7 +11433,7 @@
         <v>420</v>
       </c>
       <c r="C286" s="31" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="D286" s="29"/>
       <c r="E286" s="29" t="s">
@@ -11454,7 +11458,7 @@
         <v>420</v>
       </c>
       <c r="C287" s="31" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="D287" s="29"/>
       <c r="E287" s="29" t="s">
@@ -11479,7 +11483,7 @@
         <v>421</v>
       </c>
       <c r="C288" s="31" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="D288" s="29"/>
       <c r="E288" s="29" t="s">
@@ -11504,7 +11508,7 @@
         <v>421</v>
       </c>
       <c r="C289" s="31" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="D289" s="29"/>
       <c r="E289" s="29" t="s">
@@ -11529,7 +11533,7 @@
         <v>422</v>
       </c>
       <c r="C290" s="31" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="D290" s="29"/>
       <c r="E290" s="29" t="s">
@@ -11546,7 +11550,7 @@
       </c>
       <c r="I290" s="31"/>
     </row>
-    <row r="291" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A291" s="29" t="s">
         <v>311</v>
       </c>
@@ -11554,7 +11558,7 @@
         <v>422</v>
       </c>
       <c r="C291" s="31" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="D291" s="29"/>
       <c r="E291" s="29" t="s">
@@ -11579,7 +11583,7 @@
         <v>423</v>
       </c>
       <c r="C292" s="31" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="D292" s="29"/>
       <c r="E292" s="29" t="s">
@@ -11604,7 +11608,7 @@
         <v>424</v>
       </c>
       <c r="C293" s="31" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="D293" s="29"/>
       <c r="E293" s="29" t="s">
@@ -11629,7 +11633,7 @@
         <v>424</v>
       </c>
       <c r="C294" s="31" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="D294" s="29"/>
       <c r="E294" s="29" t="s">
@@ -11654,7 +11658,7 @@
         <v>425</v>
       </c>
       <c r="C295" s="31" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="D295" s="29"/>
       <c r="E295" s="29" t="s">
@@ -11679,7 +11683,7 @@
         <v>425</v>
       </c>
       <c r="C296" s="31" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="D296" s="29"/>
       <c r="E296" s="29" t="s">
@@ -11704,7 +11708,7 @@
         <v>425</v>
       </c>
       <c r="C297" s="31" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="D297" s="29"/>
       <c r="E297" s="29" t="s">
@@ -11729,7 +11733,7 @@
         <v>425</v>
       </c>
       <c r="C298" s="31" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="D298" s="29"/>
       <c r="E298" s="29" t="s">
@@ -11754,7 +11758,7 @@
         <v>425</v>
       </c>
       <c r="C299" s="31" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="D299" s="29"/>
       <c r="E299" s="29" t="s">
@@ -11773,13 +11777,13 @@
     </row>
     <row r="300" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A300" s="22" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="B300" s="30" t="s">
         <v>425</v>
       </c>
       <c r="C300" s="31" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="D300" s="29"/>
       <c r="E300" s="29" t="s">
@@ -11798,13 +11802,13 @@
     </row>
     <row r="301" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A301" s="22" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="B301" s="30" t="s">
         <v>425</v>
       </c>
       <c r="C301" s="20" t="s">
-        <v>866</v>
+        <v>862</v>
       </c>
       <c r="D301" s="29"/>
       <c r="E301" s="29" t="s">
@@ -11817,21 +11821,21 @@
         <v>15</v>
       </c>
       <c r="H301" s="22" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="I301" s="20" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
     </row>
     <row r="302" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A302" s="22" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="B302" s="30" t="s">
         <v>425</v>
       </c>
       <c r="C302" s="31" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="D302" s="29"/>
       <c r="E302" s="29" t="s">
@@ -11850,13 +11854,13 @@
     </row>
     <row r="303" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A303" s="22" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="B303" s="30" t="s">
         <v>425</v>
       </c>
       <c r="C303" s="31" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D303" s="29"/>
       <c r="E303" s="29" t="s">
@@ -11872,18 +11876,18 @@
         <v>17</v>
       </c>
       <c r="I303" s="31" t="s">
-        <v>816</v>
+        <v>813</v>
       </c>
     </row>
     <row r="304" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A304" s="22" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="B304" s="30" t="s">
         <v>425</v>
       </c>
       <c r="C304" s="31" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="D304" s="29"/>
       <c r="E304" s="29" t="s">
@@ -11899,18 +11903,18 @@
         <v>17</v>
       </c>
       <c r="I304" s="31" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
     </row>
     <row r="305" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A305" s="22" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="B305" s="30" t="s">
         <v>425</v>
       </c>
       <c r="C305" s="31" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="D305" s="29"/>
       <c r="E305" s="29" t="s">
@@ -11929,13 +11933,13 @@
     </row>
     <row r="306" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A306" s="22" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B306" s="30" t="s">
         <v>425</v>
       </c>
       <c r="C306" s="31" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="D306" s="29"/>
       <c r="E306" s="29" t="s">
@@ -11954,13 +11958,13 @@
     </row>
     <row r="307" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A307" s="22" t="s">
-        <v>865</v>
+        <v>861</v>
       </c>
       <c r="B307" s="30" t="s">
         <v>425</v>
       </c>
       <c r="C307" s="20" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="D307" s="29"/>
       <c r="E307" s="29" t="s">
@@ -11973,21 +11977,21 @@
         <v>15</v>
       </c>
       <c r="H307" s="22" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="I307" s="20" t="s">
-        <v>867</v>
+        <v>863</v>
       </c>
     </row>
     <row r="308" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A308" s="22" t="s">
-        <v>868</v>
+        <v>864</v>
       </c>
       <c r="B308" s="30" t="s">
         <v>425</v>
       </c>
       <c r="C308" s="20" t="s">
-        <v>878</v>
+        <v>874</v>
       </c>
       <c r="D308" s="29"/>
       <c r="E308" s="29" t="s">
@@ -12000,21 +12004,21 @@
         <v>15</v>
       </c>
       <c r="H308" s="22" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="I308" s="20" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="309" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A309" s="22" t="s">
-        <v>870</v>
+        <v>866</v>
       </c>
       <c r="B309" s="30" t="s">
         <v>425</v>
       </c>
       <c r="C309" s="31" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="D309" s="29"/>
       <c r="E309" s="29" t="s">
@@ -12039,7 +12043,7 @@
         <v>425</v>
       </c>
       <c r="C310" s="31" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="D310" s="29"/>
       <c r="E310" s="29" t="s">
@@ -12064,7 +12068,7 @@
         <v>425</v>
       </c>
       <c r="C311" s="31" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="D311" s="29"/>
       <c r="E311" s="29" t="s">
@@ -12089,7 +12093,7 @@
         <v>425</v>
       </c>
       <c r="C312" s="31" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D312" s="29"/>
       <c r="E312" s="29" t="s">
@@ -12114,7 +12118,7 @@
         <v>425</v>
       </c>
       <c r="C313" s="31" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D313" s="29"/>
       <c r="E313" s="29" t="s">
@@ -12130,7 +12134,7 @@
         <v>17</v>
       </c>
       <c r="I313" s="31" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
     <row r="314" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -12141,7 +12145,7 @@
         <v>425</v>
       </c>
       <c r="C314" s="31" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="D314" s="29"/>
       <c r="E314" s="29" t="s">
@@ -12166,7 +12170,7 @@
         <v>425</v>
       </c>
       <c r="C315" s="31" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="D315" s="29"/>
       <c r="E315" s="29" t="s">
@@ -12191,7 +12195,7 @@
         <v>425</v>
       </c>
       <c r="C316" s="31" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="D316" s="29"/>
       <c r="E316" s="29" t="s">
@@ -12207,18 +12211,18 @@
         <v>17</v>
       </c>
       <c r="I316" s="31" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
     </row>
     <row r="317" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A317" s="29" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="B317" s="30" t="s">
         <v>425</v>
       </c>
       <c r="C317" s="31" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="D317" s="29"/>
       <c r="E317" s="29" t="s">
@@ -12234,7 +12238,7 @@
         <v>17</v>
       </c>
       <c r="I317" s="31" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
     </row>
     <row r="318" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -12245,7 +12249,7 @@
         <v>425</v>
       </c>
       <c r="C318" s="31" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="D318" s="29"/>
       <c r="E318" s="29" t="s">
@@ -12270,7 +12274,7 @@
         <v>426</v>
       </c>
       <c r="C319" s="31" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="D319" s="29"/>
       <c r="E319" s="29" t="s">
@@ -12295,7 +12299,7 @@
         <v>426</v>
       </c>
       <c r="C320" s="31" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="D320" s="29"/>
       <c r="E320" s="29" t="s">
@@ -12320,7 +12324,7 @@
         <v>427</v>
       </c>
       <c r="C321" s="31" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="D321" s="29"/>
       <c r="E321" s="29" t="s">
@@ -12345,7 +12349,7 @@
         <v>427</v>
       </c>
       <c r="C322" s="31" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="D322" s="29"/>
       <c r="E322" s="29" t="s">
@@ -12370,7 +12374,7 @@
         <v>427</v>
       </c>
       <c r="C323" s="31" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="D323" s="29"/>
       <c r="E323" s="29" t="s">
@@ -12395,7 +12399,7 @@
         <v>428</v>
       </c>
       <c r="C324" s="31" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="D324" s="29"/>
       <c r="E324" s="29" t="s">
@@ -12420,7 +12424,7 @@
         <v>428</v>
       </c>
       <c r="C325" s="31" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="D325" s="29"/>
       <c r="E325" s="29" t="s">
@@ -12445,7 +12449,7 @@
         <v>429</v>
       </c>
       <c r="C326" s="31" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="D326" s="29"/>
       <c r="E326" s="29" t="s">
@@ -12470,7 +12474,7 @@
         <v>429</v>
       </c>
       <c r="C327" s="31" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="D327" s="29"/>
       <c r="E327" s="29" t="s">
@@ -12495,7 +12499,7 @@
         <v>430</v>
       </c>
       <c r="C328" s="31" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="D328" s="29"/>
       <c r="E328" s="29" t="s">
@@ -12520,7 +12524,7 @@
         <v>430</v>
       </c>
       <c r="C329" s="31" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="D329" s="29"/>
       <c r="E329" s="29" t="s">
@@ -12545,7 +12549,7 @@
         <v>430</v>
       </c>
       <c r="C330" s="31" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="D330" s="29"/>
       <c r="E330" s="29" t="s">
@@ -12570,7 +12574,7 @@
         <v>430</v>
       </c>
       <c r="C331" s="31" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="D331" s="29"/>
       <c r="E331" s="29" t="s">
@@ -12595,7 +12599,7 @@
         <v>430</v>
       </c>
       <c r="C332" s="31" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="D332" s="29"/>
       <c r="E332" s="29" t="s">
@@ -12620,7 +12624,7 @@
         <v>430</v>
       </c>
       <c r="C333" s="31" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="D333" s="29"/>
       <c r="E333" s="29" t="s">
@@ -12645,7 +12649,7 @@
         <v>430</v>
       </c>
       <c r="C334" s="31" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="D334" s="29"/>
       <c r="E334" s="29" t="s">
@@ -12670,7 +12674,7 @@
         <v>430</v>
       </c>
       <c r="C335" s="31" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="D335" s="29"/>
       <c r="E335" s="29" t="s">
@@ -12687,7 +12691,7 @@
       </c>
       <c r="I335" s="31"/>
     </row>
-    <row r="336" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A336" s="29" t="s">
         <v>345</v>
       </c>
@@ -12695,7 +12699,7 @@
         <v>430</v>
       </c>
       <c r="C336" s="31" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="D336" s="29"/>
       <c r="E336" s="29" t="s">
@@ -12720,7 +12724,7 @@
         <v>431</v>
       </c>
       <c r="C337" s="31" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="D337" s="29"/>
       <c r="E337" s="29" t="s">
@@ -12745,7 +12749,7 @@
         <v>431</v>
       </c>
       <c r="C338" s="31" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="D338" s="29"/>
       <c r="E338" s="29" t="s">
@@ -12770,7 +12774,7 @@
         <v>432</v>
       </c>
       <c r="C339" s="31" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="D339" s="29"/>
       <c r="E339" s="29" t="s">
@@ -12795,7 +12799,7 @@
         <v>432</v>
       </c>
       <c r="C340" s="31" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="D340" s="29"/>
       <c r="E340" s="29" t="s">
@@ -12820,10 +12824,10 @@
         <v>432</v>
       </c>
       <c r="C341" s="31" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="D341" s="29" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="E341" s="29" t="s">
         <v>22</v>
@@ -12838,7 +12842,7 @@
         <v>21</v>
       </c>
       <c r="I341" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="342" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -12849,7 +12853,7 @@
         <v>432</v>
       </c>
       <c r="C342" s="31" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="D342" s="29"/>
       <c r="E342" s="29" t="s">
@@ -12866,7 +12870,7 @@
       </c>
       <c r="I342" s="31"/>
     </row>
-    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A343" s="29" t="s">
         <v>352</v>
       </c>
@@ -12874,7 +12878,7 @@
         <v>432</v>
       </c>
       <c r="C343" s="31" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="D343" s="29"/>
       <c r="E343" s="29" t="s">
@@ -12899,7 +12903,7 @@
         <v>432</v>
       </c>
       <c r="C344" s="31" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="D344" s="29"/>
       <c r="E344" s="29" t="s">
@@ -12924,7 +12928,7 @@
         <v>432</v>
       </c>
       <c r="C345" s="31" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="D345" s="29"/>
       <c r="E345" s="29" t="s">
@@ -12949,10 +12953,10 @@
         <v>432</v>
       </c>
       <c r="C346" s="31" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="D346" s="29" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E346" s="29" t="s">
         <v>22</v>
@@ -12967,21 +12971,21 @@
         <v>20</v>
       </c>
       <c r="I346" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="347" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A347" s="29" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="B347" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C347" s="31" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="D347" s="29" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="E347" s="29" t="s">
         <v>22</v>
@@ -12996,7 +13000,7 @@
         <v>20</v>
       </c>
       <c r="I347" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="348" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -13007,10 +13011,10 @@
         <v>432</v>
       </c>
       <c r="C348" s="31" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D348" s="29" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="E348" s="29" t="s">
         <v>22</v>
@@ -13022,22 +13026,22 @@
         <v>15</v>
       </c>
       <c r="H348" s="29" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="I348" s="31"/>
     </row>
     <row r="349" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A349" s="29" t="s">
-        <v>822</v>
+        <v>819</v>
       </c>
       <c r="B349" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C349" s="31" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="D349" s="29" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="E349" s="29" t="s">
         <v>22</v>
@@ -13052,21 +13056,21 @@
         <v>20</v>
       </c>
       <c r="I349" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="350" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A350" s="29" t="s">
-        <v>823</v>
+        <v>820</v>
       </c>
       <c r="B350" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C350" s="31" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="D350" s="29" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="E350" s="29" t="s">
         <v>22</v>
@@ -13078,22 +13082,22 @@
         <v>15</v>
       </c>
       <c r="H350" s="29" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="I350" s="31"/>
     </row>
     <row r="351" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A351" s="29" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="B351" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C351" s="31" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="D351" s="29" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="E351" s="29" t="s">
         <v>22</v>
@@ -13108,7 +13112,7 @@
         <v>20</v>
       </c>
       <c r="I351" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="352" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -13119,10 +13123,10 @@
         <v>432</v>
       </c>
       <c r="C352" s="31" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="D352" s="29" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="E352" s="29" t="s">
         <v>22</v>
@@ -13137,21 +13141,21 @@
         <v>20</v>
       </c>
       <c r="I352" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="353" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A353" s="29" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="B353" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C353" s="31" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="D353" s="29" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="E353" s="29" t="s">
         <v>22</v>
@@ -13163,7 +13167,7 @@
         <v>15</v>
       </c>
       <c r="H353" s="29" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="I353" s="31"/>
     </row>
@@ -13175,10 +13179,10 @@
         <v>432</v>
       </c>
       <c r="C354" s="31" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="D354" s="29" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="E354" s="29" t="s">
         <v>22</v>
@@ -13193,21 +13197,21 @@
         <v>20</v>
       </c>
       <c r="I354" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="355" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A355" s="29" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="B355" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C355" s="31" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="D355" s="29" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="E355" s="29" t="s">
         <v>22</v>
@@ -13219,22 +13223,22 @@
         <v>15</v>
       </c>
       <c r="H355" s="29" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="I355" s="31"/>
     </row>
     <row r="356" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A356" s="29" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="B356" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C356" s="31" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="D356" s="29" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="E356" s="29" t="s">
         <v>22</v>
@@ -13246,22 +13250,22 @@
         <v>15</v>
       </c>
       <c r="H356" s="29" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="I356" s="31"/>
     </row>
     <row r="357" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A357" s="29" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="B357" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C357" s="31" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="D357" s="29" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="E357" s="29" t="s">
         <v>22</v>
@@ -13285,10 +13289,10 @@
         <v>432</v>
       </c>
       <c r="C358" s="31" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="D358" s="29" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="E358" s="29" t="s">
         <v>22</v>
@@ -13300,7 +13304,7 @@
         <v>15</v>
       </c>
       <c r="H358" s="29" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="I358" s="31"/>
     </row>
@@ -13312,10 +13316,10 @@
         <v>432</v>
       </c>
       <c r="C359" s="31" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="D359" s="29" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="E359" s="29" t="s">
         <v>22</v>
@@ -13333,16 +13337,16 @@
     </row>
     <row r="360" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A360" s="29" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="B360" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C360" s="31" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
       <c r="D360" s="29" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="E360" s="29" t="s">
         <v>22</v>
@@ -13354,22 +13358,22 @@
         <v>15</v>
       </c>
       <c r="H360" s="29" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="I360" s="31"/>
     </row>
     <row r="361" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A361" s="29" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="B361" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C361" s="31" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="D361" s="29" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="E361" s="29" t="s">
         <v>22</v>
@@ -13381,22 +13385,22 @@
         <v>15</v>
       </c>
       <c r="H361" s="29" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="I361" s="31"/>
     </row>
     <row r="362" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A362" s="29" t="s">
-        <v>803</v>
+        <v>800</v>
       </c>
       <c r="B362" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C362" s="31" t="s">
-        <v>801</v>
+        <v>798</v>
       </c>
       <c r="D362" s="29" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="E362" s="29" t="s">
         <v>22</v>
@@ -13408,22 +13412,22 @@
         <v>15</v>
       </c>
       <c r="H362" s="29" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="I362" s="31"/>
     </row>
     <row r="363" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A363" s="29" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="B363" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C363" s="31" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="D363" s="29" t="s">
-        <v>805</v>
+        <v>802</v>
       </c>
       <c r="E363" s="29" t="s">
         <v>22</v>
@@ -13435,7 +13439,7 @@
         <v>15</v>
       </c>
       <c r="H363" s="29" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="I363" s="31"/>
     </row>
@@ -13447,10 +13451,10 @@
         <v>432</v>
       </c>
       <c r="C364" s="31" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="D364" s="29" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="E364" s="29" t="s">
         <v>22</v>
@@ -13465,7 +13469,7 @@
         <v>20</v>
       </c>
       <c r="I364" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="365" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -13476,10 +13480,10 @@
         <v>432</v>
       </c>
       <c r="C365" s="31" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="D365" s="29" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="E365" s="29" t="s">
         <v>22</v>
@@ -13494,7 +13498,7 @@
         <v>20</v>
       </c>
       <c r="I365" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="366" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -13505,10 +13509,10 @@
         <v>432</v>
       </c>
       <c r="C366" s="31" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="D366" s="29" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="E366" s="29" t="s">
         <v>22</v>
@@ -13523,7 +13527,7 @@
         <v>20</v>
       </c>
       <c r="I366" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="367" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -13534,7 +13538,7 @@
         <v>432</v>
       </c>
       <c r="C367" s="31" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="D367" s="29"/>
       <c r="E367" s="29" t="s">
@@ -13553,16 +13557,16 @@
     </row>
     <row r="368" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A368" s="22" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="B368" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C368" s="31" t="s">
-        <v>818</v>
+        <v>815</v>
       </c>
       <c r="D368" s="22" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="E368" s="29" t="s">
         <v>22</v>
@@ -13577,47 +13581,47 @@
         <v>20</v>
       </c>
       <c r="I368" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="369" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A369" s="22" t="s">
+        <v>850</v>
+      </c>
+      <c r="B369" s="24" t="s">
+        <v>851</v>
+      </c>
+      <c r="C369" s="20" t="s">
+        <v>857</v>
+      </c>
+      <c r="D369" s="22" t="s">
+        <v>852</v>
+      </c>
+      <c r="E369" s="22" t="s">
+        <v>853</v>
+      </c>
+      <c r="F369" s="22" t="s">
         <v>854</v>
       </c>
-      <c r="B369" s="24" t="s">
+      <c r="G369" s="22" t="s">
         <v>855</v>
       </c>
-      <c r="C369" s="20" t="s">
-        <v>861</v>
-      </c>
-      <c r="D369" s="22" t="s">
+      <c r="H369" s="22" t="s">
         <v>856</v>
       </c>
-      <c r="E369" s="22" t="s">
-        <v>857</v>
-      </c>
-      <c r="F369" s="22" t="s">
-        <v>858</v>
-      </c>
-      <c r="G369" s="22" t="s">
-        <v>859</v>
-      </c>
-      <c r="H369" s="22" t="s">
-        <v>860</v>
-      </c>
       <c r="I369" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="370" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A370" s="29" t="s">
-        <v>815</v>
+        <v>812</v>
       </c>
       <c r="B370" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C370" s="31" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="D370" s="29"/>
       <c r="E370" s="29" t="s">
@@ -13636,16 +13640,16 @@
     </row>
     <row r="371" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A371" s="22" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="B371" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C371" s="31" t="s">
-        <v>820</v>
+        <v>817</v>
       </c>
       <c r="D371" s="22" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="E371" s="29" t="s">
         <v>22</v>
@@ -13660,18 +13664,18 @@
         <v>20</v>
       </c>
       <c r="I371" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="372" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A372" s="29" t="s">
-        <v>821</v>
+        <v>818</v>
       </c>
       <c r="B372" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C372" s="31" t="s">
-        <v>819</v>
+        <v>816</v>
       </c>
       <c r="D372" s="29"/>
       <c r="E372" s="29" t="s">
@@ -13688,18 +13692,18 @@
       </c>
       <c r="I372" s="31"/>
     </row>
-    <row r="373" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A373" s="22" t="s">
+        <v>867</v>
+      </c>
+      <c r="B373" s="24" t="s">
+        <v>851</v>
+      </c>
+      <c r="C373" s="20" t="s">
         <v>871</v>
       </c>
-      <c r="B373" s="24" t="s">
-        <v>855</v>
-      </c>
-      <c r="C373" s="20" t="s">
-        <v>875</v>
-      </c>
       <c r="D373" s="22" t="s">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="E373" s="29" t="s">
         <v>22</v>
@@ -13714,21 +13718,21 @@
         <v>20</v>
       </c>
       <c r="I373" s="31" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="374" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="374" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A374" s="22" t="s">
+        <v>868</v>
+      </c>
+      <c r="B374" s="24" t="s">
+        <v>851</v>
+      </c>
+      <c r="C374" s="20" t="s">
         <v>872</v>
       </c>
-      <c r="B374" s="24" t="s">
-        <v>855</v>
-      </c>
-      <c r="C374" s="20" t="s">
-        <v>876</v>
-      </c>
       <c r="D374" s="22" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
       <c r="E374" s="29" t="s">
         <v>22</v>
@@ -13743,7 +13747,7 @@
         <v>20</v>
       </c>
       <c r="I374" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="375" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -13754,10 +13758,10 @@
         <v>432</v>
       </c>
       <c r="C375" s="31" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="D375" s="29" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="E375" s="29" t="s">
         <v>22</v>
@@ -13772,7 +13776,7 @@
         <v>20</v>
       </c>
       <c r="I375" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="376" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -13783,10 +13787,10 @@
         <v>432</v>
       </c>
       <c r="C376" s="31" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="D376" s="29" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="E376" s="29" t="s">
         <v>22</v>
@@ -13801,21 +13805,21 @@
         <v>20</v>
       </c>
       <c r="I376" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="377" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A377" s="22" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="B377" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C377" s="31" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="D377" s="29" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="E377" s="29" t="s">
         <v>22</v>
@@ -13830,21 +13834,21 @@
         <v>20</v>
       </c>
       <c r="I377" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="378" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A378" s="22" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="B378" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C378" s="31" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="D378" s="22" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="E378" s="29" t="s">
         <v>22</v>
@@ -13859,21 +13863,21 @@
         <v>20</v>
       </c>
       <c r="I378" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="379" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A379" s="29" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="B379" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C379" s="31" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
       <c r="D379" s="29" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="E379" s="29" t="s">
         <v>22</v>
@@ -13888,21 +13892,21 @@
         <v>20</v>
       </c>
       <c r="I379" s="31" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
     </row>
     <row r="380" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A380" s="29" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="B380" s="30" t="s">
         <v>432</v>
       </c>
       <c r="C380" s="31" t="s">
-        <v>814</v>
+        <v>811</v>
       </c>
       <c r="D380" s="29" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="E380" s="29" t="s">
         <v>22</v>
@@ -13917,10 +13921,10 @@
         <v>20</v>
       </c>
       <c r="I380" s="31" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="381" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="381" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A381" s="29" t="s">
         <v>365</v>
       </c>
@@ -13928,7 +13932,7 @@
         <v>432</v>
       </c>
       <c r="C381" s="31" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="D381" s="29"/>
       <c r="E381" s="29" t="s">
@@ -13955,6 +13959,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -13962,11 +13971,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H304 I20:I307 A34:I381">
@@ -14030,20 +14034,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F381">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F381" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E381">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E381" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G381">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G381" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H381">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H381" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -14053,7 +14057,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B374:B383 C3 B19:B373" numberStoredAsText="1"/>
+    <ignoredError sqref="B374:B383 B19:B373" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -14063,18 +14067,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14127,6 +14131,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -14136,14 +14148,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>